<commit_message>
updated data and tcl2
</commit_message>
<xml_diff>
--- a/Project_3/data.xlsx
+++ b/Project_3/data.xlsx
@@ -1239,34 +1239,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>2.2346415294877602</c:v>
+                  <c:v>2.40772858268712</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.3097428809873302</c:v>
+                  <c:v>2.40382888512034</c:v>
                 </c:pt>
                 <c:pt idx="2" formatCode="0.00E+00">
-                  <c:v>2.1330021906447199</c:v>
+                  <c:v>2.4010104043791101</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.2488633219602998</c:v>
+                  <c:v>2.3961440432977499</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.2457785411938902</c:v>
+                  <c:v>2.3386448247934299</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.2864315785398801</c:v>
+                  <c:v>1.9716103621054999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.9250535711968799</c:v>
+                  <c:v>1.5097331919243699</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.3951168285218201</c:v>
+                  <c:v>1.0685105775080499</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.93318079725461101</c:v>
+                  <c:v>0.625007323845163</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.36093879216231101</c:v>
+                  <c:v>0.415025755405944</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1350,34 +1350,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>2.40772858268712</c:v>
+                  <c:v>2.4074556325173799</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.28022347401915</c:v>
+                  <c:v>2.4014276030405299</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.24804371981508</c:v>
+                  <c:v>2.3948106423125899</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.1560697911114302</c:v>
+                  <c:v>2.3876217050610999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.2151864270855399</c:v>
+                  <c:v>2.3380419708430802</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.0182677829721798</c:v>
+                  <c:v>1.8617380009025699</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.44247114655398101</c:v>
+                  <c:v>1.4040843303577799</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.75205598393067796</c:v>
+                  <c:v>0.90412141379983901</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.59278853018620403</c:v>
+                  <c:v>0.55883012125238096</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.546032971178539</c:v>
+                  <c:v>0.28542641071339803</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1854,34 +1854,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>6.7360939999999994E-2</c:v>
+                  <c:v>6.6047855000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.6442959999999995E-2</c:v>
+                  <c:v>6.6125630000000005E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.8512483999999998E-2</c:v>
+                  <c:v>6.6211954000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.723896E-2</c:v>
+                  <c:v>6.6333989999999995E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6.8140549999999994E-2</c:v>
+                  <c:v>6.7878530000000006E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8.8867920000000003E-2</c:v>
+                  <c:v>7.3286450000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7.4392630000000001E-2</c:v>
+                  <c:v>8.0247774999999993E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7.5352039999999995E-2</c:v>
+                  <c:v>8.5287009999999996E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8.2762290000000002E-2</c:v>
+                  <c:v>0.111540705</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.13609725</c:v>
+                  <c:v>0.14901417</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1965,34 +1965,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>6.6138169999999996E-2</c:v>
+                  <c:v>6.6073655999999995E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.6787059999999995E-2</c:v>
+                  <c:v>6.6189504999999996E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.7091410000000004E-2</c:v>
+                  <c:v>6.6297780000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.7743380000000006E-2</c:v>
+                  <c:v>6.6470840000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6.8580150000000006E-2</c:v>
+                  <c:v>6.7947074999999996E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7.0841840000000003E-2</c:v>
+                  <c:v>7.3756433999999996E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.15882569999999999</c:v>
+                  <c:v>8.0908194000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8.7833789999999995E-2</c:v>
+                  <c:v>8.617619E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9.7554624000000006E-2</c:v>
+                  <c:v>0.11435858</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.10180574000000001</c:v>
+                  <c:v>0.14842830000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2469,34 +2469,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>2.24799559658454</c:v>
+                  <c:v>2.5532883846338899</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.2472066786617999</c:v>
+                  <c:v>2.5505554074535102</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.2631953283472899</c:v>
+                  <c:v>2.54535181894718</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.2632237515609099</c:v>
+                  <c:v>2.53772691465291</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.1204710914306002</c:v>
+                  <c:v>2.4147228736378299</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.5055025603919501</c:v>
+                  <c:v>1.96151016800439</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.2612965321993901</c:v>
+                  <c:v>1.7291236438909099</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.914168188891893</c:v>
+                  <c:v>1.0736310372529201</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.52957604628694399</c:v>
+                  <c:v>0.59936217387988899</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.27388938217164899</c:v>
+                  <c:v>0.29911634894509698</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2580,34 +2580,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>2.4316434385547301</c:v>
+                  <c:v>2.5529877249322501</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.4539541012288799</c:v>
+                  <c:v>2.5477398997380298</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.4289382311113399</c:v>
+                  <c:v>2.5435855958671199</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.2553507601670102</c:v>
+                  <c:v>2.5365997228625901</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.27171020832259</c:v>
+                  <c:v>2.41243006221181</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.47742344515628</c:v>
+                  <c:v>1.95793523173706</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.5234829041597</c:v>
+                  <c:v>1.3386346607770601</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.93123644929890803</c:v>
+                  <c:v>1.0414586716202101</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.49360869878821401</c:v>
+                  <c:v>0.51741004930856604</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.34996812815148798</c:v>
+                  <c:v>0.233693339719897</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3092,34 +3092,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>6.8811916000000001E-2</c:v>
+                  <c:v>6.6098354999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.8016103999999994E-2</c:v>
+                  <c:v>6.6165940000000006E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.9036719999999996E-2</c:v>
+                  <c:v>6.6284134999999994E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.9175009999999995E-2</c:v>
+                  <c:v>6.6476720000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.2196070000000001E-2</c:v>
+                  <c:v>6.9861039999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7.7386990000000003E-2</c:v>
+                  <c:v>8.5871619999999996E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8.2277180000000005E-2</c:v>
+                  <c:v>9.7588114000000004E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9.0077005000000002E-2</c:v>
+                  <c:v>0.1128559</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.10955893</c:v>
+                  <c:v>0.13360031999999999</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.15024494999999999</c:v>
+                  <c:v>0.19120565</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3203,34 +3203,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>6.7168870000000006E-2</c:v>
+                  <c:v>6.6112526000000005E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.6645615000000005E-2</c:v>
+                  <c:v>6.6210569999999996E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.7309745000000004E-2</c:v>
+                  <c:v>6.6324279999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.8021189999999995E-2</c:v>
+                  <c:v>6.6515710000000006E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.0487270000000005E-2</c:v>
+                  <c:v>6.9903400000000004E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7.9242049999999994E-2</c:v>
+                  <c:v>8.6003010000000005E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7.9478950000000007E-2</c:v>
+                  <c:v>0.10569832</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8.9560890000000004E-2</c:v>
+                  <c:v>0.10849942999999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.11653914999999999</c:v>
+                  <c:v>0.13798622999999999</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.12874746000000001</c:v>
+                  <c:v>0.20135568000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3707,34 +3707,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>3.1347962000000001E-3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.1775457000000002E-3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.5947067999999998E-3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.5947067999999998E-3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.3185839999999999E-3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.1627907E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.4719411E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.8785983000000001E-2</c:v>
+                  <c:v>1.4023732000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>7.4226803999999993E-2</c:v>
+                  <c:v>3.0418250000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.10038610000000001</c:v>
+                  <c:v>8.66426E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3818,34 +3818,34 @@
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>9.6758589999999995E-4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.7961629999999998E-4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.4577259999999999E-3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3" formatCode="General">
-                  <c:v>2.6068822000000001E-3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4" formatCode="General">
-                  <c:v>2.072539E-3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5" formatCode="General">
-                  <c:v>1.2588513000000001E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6" formatCode="General">
-                  <c:v>1.0670732E-2</c:v>
+                  <c:v>4.3591979999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="7" formatCode="General">
-                  <c:v>2.4630540999999999E-2</c:v>
+                  <c:v>1.2331839000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="8" formatCode="General">
-                  <c:v>7.8947365000000005E-2</c:v>
+                  <c:v>5.1502145999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="9" formatCode="General">
-                  <c:v>9.9125359999999996E-2</c:v>
+                  <c:v>0.11453745</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4322,34 +4322,34 @@
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0" formatCode="General">
-                  <c:v>1.5228427E-3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.9140049999999997E-4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.6497083999999999E-3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3" formatCode="General">
-                  <c:v>1.0065425E-3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.0403223999999998E-4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5" formatCode="General">
-                  <c:v>7.0113935999999996E-3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6" formatCode="General">
-                  <c:v>6.4365129999999996E-3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7" formatCode="General">
-                  <c:v>4.0551500000000004E-3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8" formatCode="General">
-                  <c:v>1.3237064E-2</c:v>
+                  <c:v>3.5971224E-3</c:v>
                 </c:pt>
                 <c:pt idx="9" formatCode="General">
-                  <c:v>8.3333335999999994E-2</c:v>
+                  <c:v>5.1679585E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4436,31 +4436,31 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.9255590000000009E-4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2" formatCode="General">
-                  <c:v>1.0070493E-3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3" formatCode="General">
-                  <c:v>1.5797789000000001E-3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4" formatCode="General">
-                  <c:v>1.0235413999999999E-3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5" formatCode="General">
-                  <c:v>1.6797312999999999E-3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6" formatCode="General">
-                  <c:v>2.9925185999999999E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7" formatCode="General">
-                  <c:v>1.6296294999999999E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="8" formatCode="General">
-                  <c:v>3.2490975999999998E-2</c:v>
+                  <c:v>6.0362172999999996E-3</c:v>
                 </c:pt>
                 <c:pt idx="9" formatCode="General">
-                  <c:v>5.8925475999999997E-2</c:v>
+                  <c:v>4.2145595000000001E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12142,34 +12142,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>2.2231197619642402</c:v>
+                  <c:v>2.5532883846338899</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.2183411592175801</c:v>
+                  <c:v>2.5505554074535102</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.2243053710253302</c:v>
+                  <c:v>2.54535181894718</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.2265944925627301</c:v>
+                  <c:v>2.53772691465291</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.98908426244587</c:v>
+                  <c:v>2.4147228736378299</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.6476987737947</c:v>
+                  <c:v>1.96151016800439</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.4586962029983099</c:v>
+                  <c:v>1.7732462906823001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.85600971566198203</c:v>
+                  <c:v>0.79472344642503601</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.44629110210536499</c:v>
+                  <c:v>0.58968796710425198</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.24724902606898599</c:v>
+                  <c:v>0.28199545057006897</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12253,34 +12253,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>2.2375204371669701</c:v>
+                  <c:v>2.5529877249322501</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.4512907936603998</c:v>
+                  <c:v>2.5477398997380298</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.2367499785519498</c:v>
+                  <c:v>2.5435855958671199</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.1854674907709</c:v>
+                  <c:v>2.5365997228625901</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.0262822715152602</c:v>
+                  <c:v>2.41243006221181</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.14815367985956</c:v>
+                  <c:v>1.95793523173706</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.2462042583191799</c:v>
+                  <c:v>1.29528035083191</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.670968339774898</c:v>
+                  <c:v>1.0433824938435201</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.40929625706829398</c:v>
+                  <c:v>0.47560677346927099</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.32564343468812901</c:v>
+                  <c:v>0.18171930852090701</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12757,34 +12757,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>6.6833614999999999E-2</c:v>
+                  <c:v>6.6098354999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.8816749999999996E-2</c:v>
+                  <c:v>6.6165940000000006E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.8167779999999997E-2</c:v>
+                  <c:v>6.6284134999999994E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.7241850000000006E-2</c:v>
+                  <c:v>6.6476720000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.8261129999999998E-2</c:v>
+                  <c:v>6.9861039999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8.6548559999999997E-2</c:v>
+                  <c:v>8.5871619999999996E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9.5898890000000001E-2</c:v>
+                  <c:v>9.4964460000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9.9256670000000005E-2</c:v>
+                  <c:v>0.11518083</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.13313842000000001</c:v>
+                  <c:v>0.13322160999999999</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.13222893999999999</c:v>
+                  <c:v>0.17986226</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12868,34 +12868,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>6.6547549999999997E-2</c:v>
+                  <c:v>6.6112526000000005E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.7391599999999996E-2</c:v>
+                  <c:v>6.6210569999999996E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.8395499999999998E-2</c:v>
+                  <c:v>6.6324279999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.9819614000000002E-2</c:v>
+                  <c:v>6.6515710000000006E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.3262250000000001E-2</c:v>
+                  <c:v>6.9903400000000004E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8.6205299999999999E-2</c:v>
+                  <c:v>8.6003010000000005E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>9.8140249999999998E-2</c:v>
+                  <c:v>0.106187485</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.14144300000000001</c:v>
+                  <c:v>0.107535906</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.12666526</c:v>
+                  <c:v>0.1473052</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.26043077999999997</c:v>
+                  <c:v>0.23556028000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -13372,34 +13372,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>3.1678985999999999E-3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.2283297999999997E-3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.6399155999999998E-3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.1186439999999998E-3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.552398E-3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8.5409260000000008E-3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6.4102565000000002E-3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.2880214999999999E-2</c:v>
+                  <c:v>1.6011643999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>6.7599065999999999E-2</c:v>
+                  <c:v>4.2592592999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>8.6580089999999998E-2</c:v>
+                  <c:v>7.8947365000000005E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -13483,34 +13483,34 @@
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1.0515247000000001E-3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.8030738000000002E-4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2" formatCode="General">
-                  <c:v>1.5797789000000001E-3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3" formatCode="General">
-                  <c:v>2.6867276000000001E-3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4" formatCode="General">
-                  <c:v>2.8951939000000002E-3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5" formatCode="General">
-                  <c:v>1.5151516E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6" formatCode="General">
-                  <c:v>1.1669659000000001E-2</c:v>
+                  <c:v>3.6199094999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="7" formatCode="General">
-                  <c:v>3.4129694000000002E-2</c:v>
+                  <c:v>1.1173183999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="8" formatCode="General">
-                  <c:v>5.978261E-2</c:v>
+                  <c:v>5.4176073999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="9" formatCode="General">
-                  <c:v>7.6666670000000006E-2</c:v>
+                  <c:v>0.12849163</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -13997,34 +13997,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>2.24799559658454</c:v>
+                  <c:v>2.5532883846338899</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.2472066786617999</c:v>
+                  <c:v>2.5505554074535102</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.2631953283472899</c:v>
+                  <c:v>2.54535181894718</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.2632237515609099</c:v>
+                  <c:v>2.53772691465291</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.1204710914306002</c:v>
+                  <c:v>2.4147228736378299</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.5055025603919501</c:v>
+                  <c:v>1.96151016800439</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.2612965321993901</c:v>
+                  <c:v>1.7291236438909099</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.914168188891893</c:v>
+                  <c:v>1.0736310372529201</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.52957604628694399</c:v>
+                  <c:v>0.59936217387988899</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.27388938217164899</c:v>
+                  <c:v>0.29911634894509698</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -14108,34 +14108,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>2.4316434385547301</c:v>
+                  <c:v>2.5529877249322501</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.4539541012288799</c:v>
+                  <c:v>2.5477398997380298</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.4289382311113399</c:v>
+                  <c:v>2.5435855958671199</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.2553507601670102</c:v>
+                  <c:v>2.5365997228625901</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.27171020832259</c:v>
+                  <c:v>2.41243006221181</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.47742344515628</c:v>
+                  <c:v>1.95793523173706</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.5234829041597</c:v>
+                  <c:v>1.3386346607770601</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.93123644929890803</c:v>
+                  <c:v>1.0414586716202101</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.49360869878821401</c:v>
+                  <c:v>0.51741004930856604</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.34996812815148798</c:v>
+                  <c:v>0.233693339719897</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -14630,34 +14630,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>6.8811916000000001E-2</c:v>
+                  <c:v>6.6098354999999998E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.8016103999999994E-2</c:v>
+                  <c:v>6.6165940000000006E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.9036719999999996E-2</c:v>
+                  <c:v>6.6284134999999994E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.9175009999999995E-2</c:v>
+                  <c:v>6.6476720000000003E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.2196070000000001E-2</c:v>
+                  <c:v>6.9861039999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7.7386990000000003E-2</c:v>
+                  <c:v>8.5871619999999996E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8.2277180000000005E-2</c:v>
+                  <c:v>9.7588114000000004E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9.0077005000000002E-2</c:v>
+                  <c:v>0.1128559</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.10955893</c:v>
+                  <c:v>0.13360031999999999</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.15024494999999999</c:v>
+                  <c:v>0.19120565</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -14741,34 +14741,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>6.7168870000000006E-2</c:v>
+                  <c:v>6.6112526000000005E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.6645615000000005E-2</c:v>
+                  <c:v>6.6210569999999996E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>6.7309745000000004E-2</c:v>
+                  <c:v>6.6324279999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.8021189999999995E-2</c:v>
+                  <c:v>6.6515710000000006E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.0487270000000005E-2</c:v>
+                  <c:v>6.9903400000000004E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7.9242049999999994E-2</c:v>
+                  <c:v>8.6003010000000005E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>7.9478950000000007E-2</c:v>
+                  <c:v>0.10569832</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8.9560890000000004E-2</c:v>
+                  <c:v>0.10849942999999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.11653914999999999</c:v>
+                  <c:v>0.13798622999999999</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.12874746000000001</c:v>
+                  <c:v>0.20135568000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -15245,34 +15245,34 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>3.1347962000000001E-3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.1775457000000002E-3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.5947067999999998E-3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.5947067999999998E-3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.3185839999999999E-3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.1627907E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.4719411E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2.8785983000000001E-2</c:v>
+                  <c:v>1.4023732000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>7.4226803999999993E-2</c:v>
+                  <c:v>3.0418250000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.10038610000000001</c:v>
+                  <c:v>8.66426E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -15356,34 +15356,34 @@
                 <c:formatCode>0.00E+00</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>9.6758589999999995E-4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.7961629999999998E-4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.4577259999999999E-3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="3" formatCode="General">
-                  <c:v>2.6068822000000001E-3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="4" formatCode="General">
-                  <c:v>2.072539E-3</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="5" formatCode="General">
-                  <c:v>1.2588513000000001E-2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="6" formatCode="General">
-                  <c:v>1.0670732E-2</c:v>
+                  <c:v>4.3591979999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="7" formatCode="General">
-                  <c:v>2.4630540999999999E-2</c:v>
+                  <c:v>1.2331839000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="8" formatCode="General">
-                  <c:v>7.8947365000000005E-2</c:v>
+                  <c:v>5.1502145999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="9" formatCode="General">
-                  <c:v>9.9125359999999996E-2</c:v>
+                  <c:v>0.11453745</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -28809,8 +28809,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="P132" sqref="P132"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="E69" sqref="E69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -29398,34 +29398,34 @@
         <v>9</v>
       </c>
       <c r="B23">
-        <v>2.2231197619642402</v>
+        <v>2.5532883846338899</v>
       </c>
       <c r="C23">
-        <v>2.2183411592175801</v>
+        <v>2.5505554074535102</v>
       </c>
       <c r="D23">
-        <v>2.2243053710253302</v>
+        <v>2.54535181894718</v>
       </c>
       <c r="E23">
-        <v>2.2265944925627301</v>
+        <v>2.53772691465291</v>
       </c>
       <c r="F23">
-        <v>1.98908426244587</v>
+        <v>2.4147228736378299</v>
       </c>
       <c r="G23">
-        <v>1.6476987737947</v>
+        <v>1.96151016800439</v>
       </c>
       <c r="H23">
-        <v>1.4586962029983099</v>
+        <v>1.7732462906823001</v>
       </c>
       <c r="I23">
-        <v>0.85600971566198203</v>
+        <v>0.79472344642503601</v>
       </c>
       <c r="J23">
-        <v>0.44629110210536499</v>
+        <v>0.58968796710425198</v>
       </c>
       <c r="K23">
-        <v>0.24724902606898599</v>
+        <v>0.28199545057006897</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
@@ -29433,34 +29433,34 @@
         <v>10</v>
       </c>
       <c r="B24">
-        <v>2.2375204371669701</v>
+        <v>2.5529877249322501</v>
       </c>
       <c r="C24">
-        <v>2.4512907936603998</v>
+        <v>2.5477398997380298</v>
       </c>
       <c r="D24">
-        <v>2.2367499785519498</v>
+        <v>2.5435855958671199</v>
       </c>
       <c r="E24">
-        <v>2.1854674907709</v>
+        <v>2.5365997228625901</v>
       </c>
       <c r="F24">
-        <v>2.0262822715152602</v>
+        <v>2.41243006221181</v>
       </c>
       <c r="G24">
-        <v>1.14815367985956</v>
+        <v>1.95793523173706</v>
       </c>
       <c r="H24">
-        <v>1.2462042583191799</v>
+        <v>1.29528035083191</v>
       </c>
       <c r="I24">
-        <v>0.670968339774898</v>
+        <v>1.0433824938435201</v>
       </c>
       <c r="J24">
-        <v>0.40929625706829398</v>
+        <v>0.47560677346927099</v>
       </c>
       <c r="K24">
-        <v>0.32564343468812901</v>
+        <v>0.18171930852090701</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
@@ -29503,34 +29503,34 @@
         <v>9</v>
       </c>
       <c r="B27">
-        <v>6.6833614999999999E-2</v>
+        <v>6.6098354999999998E-2</v>
       </c>
       <c r="C27">
-        <v>6.8816749999999996E-2</v>
+        <v>6.6165940000000006E-2</v>
       </c>
       <c r="D27">
-        <v>6.8167779999999997E-2</v>
+        <v>6.6284134999999994E-2</v>
       </c>
       <c r="E27">
-        <v>6.7241850000000006E-2</v>
+        <v>6.6476720000000003E-2</v>
       </c>
       <c r="F27">
-        <v>7.8261129999999998E-2</v>
+        <v>6.9861039999999999E-2</v>
       </c>
       <c r="G27">
-        <v>8.6548559999999997E-2</v>
+        <v>8.5871619999999996E-2</v>
       </c>
       <c r="H27">
-        <v>9.5898890000000001E-2</v>
+        <v>9.4964460000000001E-2</v>
       </c>
       <c r="I27">
-        <v>9.9256670000000005E-2</v>
+        <v>0.11518083</v>
       </c>
       <c r="J27">
-        <v>0.13313842000000001</v>
+        <v>0.13322160999999999</v>
       </c>
       <c r="K27">
-        <v>0.13222893999999999</v>
+        <v>0.17986226</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
@@ -29538,34 +29538,34 @@
         <v>10</v>
       </c>
       <c r="B28">
-        <v>6.6547549999999997E-2</v>
+        <v>6.6112526000000005E-2</v>
       </c>
       <c r="C28">
-        <v>6.7391599999999996E-2</v>
+        <v>6.6210569999999996E-2</v>
       </c>
       <c r="D28">
-        <v>6.8395499999999998E-2</v>
+        <v>6.6324279999999999E-2</v>
       </c>
       <c r="E28">
-        <v>6.9819614000000002E-2</v>
+        <v>6.6515710000000006E-2</v>
       </c>
       <c r="F28">
-        <v>7.3262250000000001E-2</v>
+        <v>6.9903400000000004E-2</v>
       </c>
       <c r="G28">
-        <v>8.6205299999999999E-2</v>
+        <v>8.6003010000000005E-2</v>
       </c>
       <c r="H28">
-        <v>9.8140249999999998E-2</v>
+        <v>0.106187485</v>
       </c>
       <c r="I28">
-        <v>0.14144300000000001</v>
+        <v>0.107535906</v>
       </c>
       <c r="J28">
-        <v>0.12666526</v>
+        <v>0.1473052</v>
       </c>
       <c r="K28">
-        <v>0.26043077999999997</v>
+        <v>0.23556028000000001</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
@@ -29608,34 +29608,34 @@
         <v>9</v>
       </c>
       <c r="B31">
-        <v>3.1678985999999999E-3</v>
+        <v>0</v>
       </c>
       <c r="C31">
-        <v>4.2283297999999997E-3</v>
+        <v>0</v>
       </c>
       <c r="D31">
-        <v>2.6399155999999998E-3</v>
+        <v>0</v>
       </c>
       <c r="E31">
-        <v>2.1186439999999998E-3</v>
+        <v>0</v>
       </c>
       <c r="F31">
-        <v>3.552398E-3</v>
+        <v>0</v>
       </c>
       <c r="G31">
-        <v>8.5409260000000008E-3</v>
+        <v>0</v>
       </c>
       <c r="H31">
-        <v>6.4102565000000002E-3</v>
+        <v>0</v>
       </c>
       <c r="I31">
-        <v>2.2880214999999999E-2</v>
+        <v>1.6011643999999998E-2</v>
       </c>
       <c r="J31">
-        <v>6.7599065999999999E-2</v>
+        <v>4.2592592999999998E-2</v>
       </c>
       <c r="K31">
-        <v>8.6580089999999998E-2</v>
+        <v>7.8947365000000005E-2</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
@@ -29643,34 +29643,34 @@
         <v>10</v>
       </c>
       <c r="B32" s="4">
-        <v>1.0515247000000001E-3</v>
+        <v>0</v>
       </c>
       <c r="C32" s="4">
-        <v>4.8030738000000002E-4</v>
+        <v>0</v>
       </c>
       <c r="D32">
-        <v>1.5797789000000001E-3</v>
+        <v>0</v>
       </c>
       <c r="E32">
-        <v>2.6867276000000001E-3</v>
+        <v>0</v>
       </c>
       <c r="F32">
-        <v>2.8951939000000002E-3</v>
+        <v>0</v>
       </c>
       <c r="G32">
-        <v>1.5151516E-2</v>
+        <v>0</v>
       </c>
       <c r="H32">
-        <v>1.1669659000000001E-2</v>
+        <v>3.6199094999999999E-3</v>
       </c>
       <c r="I32">
-        <v>3.4129694000000002E-2</v>
+        <v>1.1173183999999999E-2</v>
       </c>
       <c r="J32">
-        <v>5.978261E-2</v>
+        <v>5.4176073999999998E-2</v>
       </c>
       <c r="K32">
-        <v>7.6666670000000006E-2</v>
+        <v>0.12849163</v>
       </c>
     </row>
     <row r="33" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -29719,34 +29719,34 @@
         <v>11</v>
       </c>
       <c r="B36">
-        <v>2.24799559658454</v>
+        <v>2.5532883846338899</v>
       </c>
       <c r="C36">
-        <v>2.2472066786617999</v>
+        <v>2.5505554074535102</v>
       </c>
       <c r="D36">
-        <v>2.2631953283472899</v>
+        <v>2.54535181894718</v>
       </c>
       <c r="E36">
-        <v>2.2632237515609099</v>
+        <v>2.53772691465291</v>
       </c>
       <c r="F36">
-        <v>2.1204710914306002</v>
+        <v>2.4147228736378299</v>
       </c>
       <c r="G36">
-        <v>1.5055025603919501</v>
+        <v>1.96151016800439</v>
       </c>
       <c r="H36">
-        <v>1.2612965321993901</v>
+        <v>1.7291236438909099</v>
       </c>
       <c r="I36">
-        <v>0.914168188891893</v>
+        <v>1.0736310372529201</v>
       </c>
       <c r="J36">
-        <v>0.52957604628694399</v>
+        <v>0.59936217387988899</v>
       </c>
       <c r="K36">
-        <v>0.27388938217164899</v>
+        <v>0.29911634894509698</v>
       </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
@@ -29754,34 +29754,34 @@
         <v>1</v>
       </c>
       <c r="B37">
-        <v>2.4316434385547301</v>
+        <v>2.5529877249322501</v>
       </c>
       <c r="C37">
-        <v>2.4539541012288799</v>
+        <v>2.5477398997380298</v>
       </c>
       <c r="D37">
-        <v>2.4289382311113399</v>
+        <v>2.5435855958671199</v>
       </c>
       <c r="E37">
-        <v>2.2553507601670102</v>
+        <v>2.5365997228625901</v>
       </c>
       <c r="F37">
-        <v>2.27171020832259</v>
+        <v>2.41243006221181</v>
       </c>
       <c r="G37">
-        <v>1.47742344515628</v>
+        <v>1.95793523173706</v>
       </c>
       <c r="H37">
-        <v>1.5234829041597</v>
+        <v>1.3386346607770601</v>
       </c>
       <c r="I37">
-        <v>0.93123644929890803</v>
+        <v>1.0414586716202101</v>
       </c>
       <c r="J37">
-        <v>0.49360869878821401</v>
+        <v>0.51741004930856604</v>
       </c>
       <c r="K37">
-        <v>0.34996812815148798</v>
+        <v>0.233693339719897</v>
       </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
@@ -29824,34 +29824,34 @@
         <v>11</v>
       </c>
       <c r="B40">
-        <v>6.8811916000000001E-2</v>
+        <v>6.6098354999999998E-2</v>
       </c>
       <c r="C40">
-        <v>6.8016103999999994E-2</v>
+        <v>6.6165940000000006E-2</v>
       </c>
       <c r="D40">
-        <v>6.9036719999999996E-2</v>
+        <v>6.6284134999999994E-2</v>
       </c>
       <c r="E40">
-        <v>6.9175009999999995E-2</v>
+        <v>6.6476720000000003E-2</v>
       </c>
       <c r="F40">
-        <v>7.2196070000000001E-2</v>
+        <v>6.9861039999999999E-2</v>
       </c>
       <c r="G40">
-        <v>7.7386990000000003E-2</v>
+        <v>8.5871619999999996E-2</v>
       </c>
       <c r="H40">
-        <v>8.2277180000000005E-2</v>
+        <v>9.7588114000000004E-2</v>
       </c>
       <c r="I40">
-        <v>9.0077005000000002E-2</v>
+        <v>0.1128559</v>
       </c>
       <c r="J40">
-        <v>0.10955893</v>
+        <v>0.13360031999999999</v>
       </c>
       <c r="K40">
-        <v>0.15024494999999999</v>
+        <v>0.19120565</v>
       </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
@@ -29859,34 +29859,34 @@
         <v>1</v>
       </c>
       <c r="B41">
-        <v>6.7168870000000006E-2</v>
+        <v>6.6112526000000005E-2</v>
       </c>
       <c r="C41">
-        <v>6.6645615000000005E-2</v>
+        <v>6.6210569999999996E-2</v>
       </c>
       <c r="D41">
-        <v>6.7309745000000004E-2</v>
+        <v>6.6324279999999999E-2</v>
       </c>
       <c r="E41">
-        <v>6.8021189999999995E-2</v>
+        <v>6.6515710000000006E-2</v>
       </c>
       <c r="F41">
-        <v>7.0487270000000005E-2</v>
+        <v>6.9903400000000004E-2</v>
       </c>
       <c r="G41">
-        <v>7.9242049999999994E-2</v>
+        <v>8.6003010000000005E-2</v>
       </c>
       <c r="H41">
-        <v>7.9478950000000007E-2</v>
+        <v>0.10569832</v>
       </c>
       <c r="I41">
-        <v>8.9560890000000004E-2</v>
+        <v>0.10849942999999999</v>
       </c>
       <c r="J41">
-        <v>0.11653914999999999</v>
+        <v>0.13798622999999999</v>
       </c>
       <c r="K41">
-        <v>0.12874746000000001</v>
+        <v>0.20135568000000001</v>
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
@@ -29929,34 +29929,34 @@
         <v>11</v>
       </c>
       <c r="B44">
-        <v>3.1347962000000001E-3</v>
+        <v>0</v>
       </c>
       <c r="C44">
-        <v>4.1775457000000002E-3</v>
+        <v>0</v>
       </c>
       <c r="D44">
-        <v>2.5947067999999998E-3</v>
+        <v>0</v>
       </c>
       <c r="E44">
-        <v>2.5947067999999998E-3</v>
+        <v>0</v>
       </c>
       <c r="F44">
-        <v>3.3185839999999999E-3</v>
+        <v>0</v>
       </c>
       <c r="G44">
-        <v>1.1627907E-2</v>
+        <v>0</v>
       </c>
       <c r="H44">
-        <v>1.4719411E-2</v>
+        <v>0</v>
       </c>
       <c r="I44">
-        <v>2.8785983000000001E-2</v>
+        <v>1.4023732000000001E-2</v>
       </c>
       <c r="J44">
-        <v>7.4226803999999993E-2</v>
+        <v>3.0418250000000001E-2</v>
       </c>
       <c r="K44">
-        <v>0.10038610000000001</v>
+        <v>8.66426E-2</v>
       </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.25">
@@ -29964,34 +29964,34 @@
         <v>1</v>
       </c>
       <c r="B45" s="4">
-        <v>9.6758589999999995E-4</v>
+        <v>0</v>
       </c>
       <c r="C45" s="4">
-        <v>4.7961629999999998E-4</v>
+        <v>0</v>
       </c>
       <c r="D45" s="4">
-        <v>1.4577259999999999E-3</v>
+        <v>0</v>
       </c>
       <c r="E45">
-        <v>2.6068822000000001E-3</v>
+        <v>0</v>
       </c>
       <c r="F45">
-        <v>2.072539E-3</v>
+        <v>0</v>
       </c>
       <c r="G45">
-        <v>1.2588513000000001E-2</v>
+        <v>0</v>
       </c>
       <c r="H45">
-        <v>1.0670732E-2</v>
+        <v>4.3591979999999999E-3</v>
       </c>
       <c r="I45">
-        <v>2.4630540999999999E-2</v>
+        <v>1.2331839000000001E-2</v>
       </c>
       <c r="J45">
-        <v>7.8947365000000005E-2</v>
+        <v>5.1502145999999999E-2</v>
       </c>
       <c r="K45">
-        <v>9.9125359999999996E-2</v>
+        <v>0.11453745</v>
       </c>
     </row>
     <row r="46" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -30044,34 +30044,34 @@
         <v>16</v>
       </c>
       <c r="B49">
-        <v>2.2346415294877602</v>
+        <v>2.40772858268712</v>
       </c>
       <c r="C49">
-        <v>2.3097428809873302</v>
+        <v>2.40382888512034</v>
       </c>
       <c r="D49" s="4">
-        <v>2.1330021906447199</v>
+        <v>2.4010104043791101</v>
       </c>
       <c r="E49">
-        <v>2.2488633219602998</v>
+        <v>2.3961440432977499</v>
       </c>
       <c r="F49">
-        <v>2.2457785411938902</v>
+        <v>2.3386448247934299</v>
       </c>
       <c r="G49">
-        <v>1.2864315785398801</v>
+        <v>1.9716103621054999</v>
       </c>
       <c r="H49">
-        <v>1.9250535711968799</v>
+        <v>1.5097331919243699</v>
       </c>
       <c r="I49">
-        <v>1.3951168285218201</v>
+        <v>1.0685105775080499</v>
       </c>
       <c r="J49">
-        <v>0.93318079725461101</v>
+        <v>0.625007323845163</v>
       </c>
       <c r="K49">
-        <v>0.36093879216231101</v>
+        <v>0.415025755405944</v>
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
@@ -30079,34 +30079,34 @@
         <v>17</v>
       </c>
       <c r="B50">
-        <v>2.40772858268712</v>
+        <v>2.4074556325173799</v>
       </c>
       <c r="C50">
-        <v>2.28022347401915</v>
+        <v>2.4014276030405299</v>
       </c>
       <c r="D50">
-        <v>2.24804371981508</v>
+        <v>2.3948106423125899</v>
       </c>
       <c r="E50">
-        <v>2.1560697911114302</v>
+        <v>2.3876217050610999</v>
       </c>
       <c r="F50">
-        <v>2.2151864270855399</v>
+        <v>2.3380419708430802</v>
       </c>
       <c r="G50">
-        <v>2.0182677829721798</v>
+        <v>1.8617380009025699</v>
       </c>
       <c r="H50">
-        <v>0.44247114655398101</v>
+        <v>1.4040843303577799</v>
       </c>
       <c r="I50">
-        <v>0.75205598393067796</v>
+        <v>0.90412141379983901</v>
       </c>
       <c r="J50">
-        <v>0.59278853018620403</v>
+        <v>0.55883012125238096</v>
       </c>
       <c r="K50">
-        <v>0.546032971178539</v>
+        <v>0.28542641071339803</v>
       </c>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.25">
@@ -30149,34 +30149,34 @@
         <v>16</v>
       </c>
       <c r="B53">
-        <v>6.7360939999999994E-2</v>
+        <v>6.6047855000000003E-2</v>
       </c>
       <c r="C53">
-        <v>6.6442959999999995E-2</v>
+        <v>6.6125630000000005E-2</v>
       </c>
       <c r="D53">
-        <v>6.8512483999999998E-2</v>
+        <v>6.6211954000000003E-2</v>
       </c>
       <c r="E53">
-        <v>6.723896E-2</v>
+        <v>6.6333989999999995E-2</v>
       </c>
       <c r="F53">
-        <v>6.8140549999999994E-2</v>
+        <v>6.7878530000000006E-2</v>
       </c>
       <c r="G53">
-        <v>8.8867920000000003E-2</v>
+        <v>7.3286450000000003E-2</v>
       </c>
       <c r="H53">
-        <v>7.4392630000000001E-2</v>
+        <v>8.0247774999999993E-2</v>
       </c>
       <c r="I53">
-        <v>7.5352039999999995E-2</v>
+        <v>8.5287009999999996E-2</v>
       </c>
       <c r="J53">
-        <v>8.2762290000000002E-2</v>
+        <v>0.111540705</v>
       </c>
       <c r="K53">
-        <v>0.13609725</v>
+        <v>0.14901417</v>
       </c>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.25">
@@ -30184,34 +30184,34 @@
         <v>17</v>
       </c>
       <c r="B54">
-        <v>6.6138169999999996E-2</v>
+        <v>6.6073655999999995E-2</v>
       </c>
       <c r="C54">
-        <v>6.6787059999999995E-2</v>
+        <v>6.6189504999999996E-2</v>
       </c>
       <c r="D54">
-        <v>6.7091410000000004E-2</v>
+        <v>6.6297780000000001E-2</v>
       </c>
       <c r="E54">
-        <v>6.7743380000000006E-2</v>
+        <v>6.6470840000000003E-2</v>
       </c>
       <c r="F54">
-        <v>6.8580150000000006E-2</v>
+        <v>6.7947074999999996E-2</v>
       </c>
       <c r="G54">
-        <v>7.0841840000000003E-2</v>
+        <v>7.3756433999999996E-2</v>
       </c>
       <c r="H54">
-        <v>0.15882569999999999</v>
+        <v>8.0908194000000003E-2</v>
       </c>
       <c r="I54">
-        <v>8.7833789999999995E-2</v>
+        <v>8.617619E-2</v>
       </c>
       <c r="J54">
-        <v>9.7554624000000006E-2</v>
+        <v>0.11435858</v>
       </c>
       <c r="K54">
-        <v>0.10180574000000001</v>
+        <v>0.14842830000000001</v>
       </c>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.25">
@@ -30254,34 +30254,34 @@
         <v>16</v>
       </c>
       <c r="B57">
-        <v>1.5228427E-3</v>
+        <v>0</v>
       </c>
       <c r="C57" s="4">
-        <v>4.9140049999999997E-4</v>
+        <v>0</v>
       </c>
       <c r="D57" s="4">
-        <v>2.6497083999999999E-3</v>
+        <v>0</v>
       </c>
       <c r="E57">
-        <v>1.0065425E-3</v>
+        <v>0</v>
       </c>
       <c r="F57" s="4">
-        <v>5.0403223999999998E-4</v>
+        <v>0</v>
       </c>
       <c r="G57">
-        <v>7.0113935999999996E-3</v>
+        <v>0</v>
       </c>
       <c r="H57">
-        <v>6.4365129999999996E-3</v>
+        <v>0</v>
       </c>
       <c r="I57">
-        <v>4.0551500000000004E-3</v>
+        <v>0</v>
       </c>
       <c r="J57">
-        <v>1.3237064E-2</v>
+        <v>3.5971224E-3</v>
       </c>
       <c r="K57">
-        <v>8.3333335999999994E-2</v>
+        <v>5.1679585E-2</v>
       </c>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
@@ -30292,31 +30292,31 @@
         <v>0</v>
       </c>
       <c r="C58" s="4">
-        <v>9.9255590000000009E-4</v>
+        <v>0</v>
       </c>
       <c r="D58">
-        <v>1.0070493E-3</v>
+        <v>0</v>
       </c>
       <c r="E58">
-        <v>1.5797789000000001E-3</v>
+        <v>0</v>
       </c>
       <c r="F58">
-        <v>1.0235413999999999E-3</v>
+        <v>0</v>
       </c>
       <c r="G58">
-        <v>1.6797312999999999E-3</v>
+        <v>0</v>
       </c>
       <c r="H58">
-        <v>2.9925185999999999E-2</v>
+        <v>0</v>
       </c>
       <c r="I58">
-        <v>1.6296294999999999E-2</v>
+        <v>0</v>
       </c>
       <c r="J58">
-        <v>3.2490975999999998E-2</v>
+        <v>6.0362172999999996E-3</v>
       </c>
       <c r="K58">
-        <v>5.8925475999999997E-2</v>
+        <v>4.2145595000000001E-2</v>
       </c>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.25">
@@ -30374,34 +30374,34 @@
         <v>11</v>
       </c>
       <c r="B63">
-        <v>2.24799559658454</v>
+        <v>2.5532883846338899</v>
       </c>
       <c r="C63">
-        <v>2.2472066786617999</v>
+        <v>2.5505554074535102</v>
       </c>
       <c r="D63">
-        <v>2.2631953283472899</v>
+        <v>2.54535181894718</v>
       </c>
       <c r="E63">
-        <v>2.2632237515609099</v>
+        <v>2.53772691465291</v>
       </c>
       <c r="F63">
-        <v>2.1204710914306002</v>
+        <v>2.4147228736378299</v>
       </c>
       <c r="G63">
-        <v>1.5055025603919501</v>
+        <v>1.96151016800439</v>
       </c>
       <c r="H63">
-        <v>1.2612965321993901</v>
+        <v>1.7291236438909099</v>
       </c>
       <c r="I63">
-        <v>0.914168188891893</v>
+        <v>1.0736310372529201</v>
       </c>
       <c r="J63">
-        <v>0.52957604628694399</v>
+        <v>0.59936217387988899</v>
       </c>
       <c r="K63">
-        <v>0.27388938217164899</v>
+        <v>0.29911634894509698</v>
       </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.25">
@@ -30409,34 +30409,34 @@
         <v>3</v>
       </c>
       <c r="B64">
-        <v>2.4316434385547301</v>
+        <v>2.5529877249322501</v>
       </c>
       <c r="C64">
-        <v>2.4539541012288799</v>
+        <v>2.5477398997380298</v>
       </c>
       <c r="D64">
-        <v>2.4289382311113399</v>
+        <v>2.5435855958671199</v>
       </c>
       <c r="E64">
-        <v>2.2553507601670102</v>
+        <v>2.5365997228625901</v>
       </c>
       <c r="F64">
-        <v>2.27171020832259</v>
+        <v>2.41243006221181</v>
       </c>
       <c r="G64">
-        <v>1.47742344515628</v>
+        <v>1.95793523173706</v>
       </c>
       <c r="H64">
-        <v>1.5234829041597</v>
+        <v>1.3386346607770601</v>
       </c>
       <c r="I64">
-        <v>0.93123644929890803</v>
+        <v>1.0414586716202101</v>
       </c>
       <c r="J64">
-        <v>0.49360869878821401</v>
+        <v>0.51741004930856604</v>
       </c>
       <c r="K64">
-        <v>0.34996812815148798</v>
+        <v>0.233693339719897</v>
       </c>
     </row>
     <row r="66" spans="1:36" x14ac:dyDescent="0.25">
@@ -30479,34 +30479,34 @@
         <v>11</v>
       </c>
       <c r="B67">
-        <v>6.8811916000000001E-2</v>
+        <v>6.6098354999999998E-2</v>
       </c>
       <c r="C67">
-        <v>6.8016103999999994E-2</v>
+        <v>6.6165940000000006E-2</v>
       </c>
       <c r="D67">
-        <v>6.9036719999999996E-2</v>
+        <v>6.6284134999999994E-2</v>
       </c>
       <c r="E67">
-        <v>6.9175009999999995E-2</v>
+        <v>6.6476720000000003E-2</v>
       </c>
       <c r="F67">
-        <v>7.2196070000000001E-2</v>
+        <v>6.9861039999999999E-2</v>
       </c>
       <c r="G67">
-        <v>7.7386990000000003E-2</v>
+        <v>8.5871619999999996E-2</v>
       </c>
       <c r="H67">
-        <v>8.2277180000000005E-2</v>
+        <v>9.7588114000000004E-2</v>
       </c>
       <c r="I67">
-        <v>9.0077005000000002E-2</v>
+        <v>0.1128559</v>
       </c>
       <c r="J67">
-        <v>0.10955893</v>
+        <v>0.13360031999999999</v>
       </c>
       <c r="K67">
-        <v>0.15024494999999999</v>
+        <v>0.19120565</v>
       </c>
     </row>
     <row r="68" spans="1:36" x14ac:dyDescent="0.25">
@@ -30514,34 +30514,34 @@
         <v>3</v>
       </c>
       <c r="B68">
-        <v>6.7168870000000006E-2</v>
+        <v>6.6112526000000005E-2</v>
       </c>
       <c r="C68">
-        <v>6.6645615000000005E-2</v>
+        <v>6.6210569999999996E-2</v>
       </c>
       <c r="D68">
-        <v>6.7309745000000004E-2</v>
+        <v>6.6324279999999999E-2</v>
       </c>
       <c r="E68">
-        <v>6.8021189999999995E-2</v>
+        <v>6.6515710000000006E-2</v>
       </c>
       <c r="F68">
-        <v>7.0487270000000005E-2</v>
+        <v>6.9903400000000004E-2</v>
       </c>
       <c r="G68">
-        <v>7.9242049999999994E-2</v>
+        <v>8.6003010000000005E-2</v>
       </c>
       <c r="H68">
-        <v>7.9478950000000007E-2</v>
+        <v>0.10569832</v>
       </c>
       <c r="I68">
-        <v>8.9560890000000004E-2</v>
+        <v>0.10849942999999999</v>
       </c>
       <c r="J68">
-        <v>0.11653914999999999</v>
+        <v>0.13798622999999999</v>
       </c>
       <c r="K68">
-        <v>0.12874746000000001</v>
+        <v>0.20135568000000001</v>
       </c>
     </row>
     <row r="70" spans="1:36" x14ac:dyDescent="0.25">
@@ -30584,34 +30584,34 @@
         <v>11</v>
       </c>
       <c r="B71">
-        <v>3.1347962000000001E-3</v>
+        <v>0</v>
       </c>
       <c r="C71">
-        <v>4.1775457000000002E-3</v>
+        <v>0</v>
       </c>
       <c r="D71">
-        <v>2.5947067999999998E-3</v>
+        <v>0</v>
       </c>
       <c r="E71">
-        <v>2.5947067999999998E-3</v>
+        <v>0</v>
       </c>
       <c r="F71">
-        <v>3.3185839999999999E-3</v>
+        <v>0</v>
       </c>
       <c r="G71">
-        <v>1.1627907E-2</v>
+        <v>0</v>
       </c>
       <c r="H71">
-        <v>1.4719411E-2</v>
+        <v>0</v>
       </c>
       <c r="I71">
-        <v>2.8785983000000001E-2</v>
+        <v>1.4023732000000001E-2</v>
       </c>
       <c r="J71">
-        <v>7.4226803999999993E-2</v>
+        <v>3.0418250000000001E-2</v>
       </c>
       <c r="K71">
-        <v>0.10038610000000001</v>
+        <v>8.66426E-2</v>
       </c>
     </row>
     <row r="72" spans="1:36" x14ac:dyDescent="0.25">
@@ -30619,34 +30619,34 @@
         <v>3</v>
       </c>
       <c r="B72" s="4">
-        <v>9.6758589999999995E-4</v>
+        <v>0</v>
       </c>
       <c r="C72" s="4">
-        <v>4.7961629999999998E-4</v>
+        <v>0</v>
       </c>
       <c r="D72" s="4">
-        <v>1.4577259999999999E-3</v>
+        <v>0</v>
       </c>
       <c r="E72">
-        <v>2.6068822000000001E-3</v>
+        <v>0</v>
       </c>
       <c r="F72">
-        <v>2.072539E-3</v>
+        <v>0</v>
       </c>
       <c r="G72">
-        <v>1.2588513000000001E-2</v>
+        <v>0</v>
       </c>
       <c r="H72">
-        <v>1.0670732E-2</v>
+        <v>4.3591979999999999E-3</v>
       </c>
       <c r="I72">
-        <v>2.4630540999999999E-2</v>
+        <v>1.2331839000000001E-2</v>
       </c>
       <c r="J72">
-        <v>7.8947365000000005E-2</v>
+        <v>5.1502145999999999E-2</v>
       </c>
       <c r="K72">
-        <v>9.9125359999999996E-2</v>
+        <v>0.11453745</v>
       </c>
     </row>
     <row r="74" spans="1:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
update start time and data
</commit_message>
<xml_diff>
--- a/Project_3/data.xlsx
+++ b/Project_3/data.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="25">
   <si>
     <t>Tahoe</t>
   </si>
@@ -234,7 +234,7 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
@@ -251,6 +251,10 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="11" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -27707,8 +27711,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ100"/>
   <sheetViews>
-    <sheetView topLeftCell="N73" workbookViewId="0">
-      <selection activeCell="A76" sqref="A76:AJ78"/>
+    <sheetView topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="A62" sqref="A62:K64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -31553,16 +31557,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q52"/>
+  <dimension ref="A1:S69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="S66" sqref="S66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="11" max="12" width="10.140625" bestFit="1" customWidth="1"/>
     <col min="14" max="17" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="12.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
@@ -31969,7 +31974,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>1</v>
       </c>
@@ -31995,7 +32000,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>1.25</v>
       </c>
@@ -32033,7 +32038,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>1.5</v>
       </c>
@@ -32071,7 +32076,7 @@
         <v>1.8419999999999999E-11</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>1.75</v>
       </c>
@@ -32109,7 +32114,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2</v>
       </c>
@@ -32129,7 +32134,7 @@
         <v>0.64572143999999998</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>2.25</v>
       </c>
@@ -32149,7 +32154,7 @@
         <v>0.19783816000000001</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>2.5</v>
       </c>
@@ -32168,8 +32173,35 @@
       <c r="G23">
         <v>0.68800455000000005</v>
       </c>
+      <c r="I23" t="s">
+        <v>5</v>
+      </c>
+      <c r="J23" t="s">
+        <v>9</v>
+      </c>
+      <c r="K23" t="s">
+        <v>10</v>
+      </c>
+      <c r="M23" t="s">
+        <v>23</v>
+      </c>
+      <c r="N23" t="s">
+        <v>9</v>
+      </c>
+      <c r="O23" t="s">
+        <v>10</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>24</v>
+      </c>
+      <c r="R23" t="s">
+        <v>9</v>
+      </c>
+      <c r="S23" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>2.75</v>
       </c>
@@ -32188,8 +32220,35 @@
       <c r="G24">
         <v>1.0750082999999999</v>
       </c>
+      <c r="I24">
+        <v>1</v>
+      </c>
+      <c r="J24">
+        <v>2.5532883846338899</v>
+      </c>
+      <c r="K24">
+        <v>2.5529877249322501</v>
+      </c>
+      <c r="M24" t="s">
+        <v>9</v>
+      </c>
+      <c r="N24" s="10">
+        <v>0</v>
+      </c>
+      <c r="O24" s="10">
+        <v>34.344999999999999</v>
+      </c>
+      <c r="Q24" t="s">
+        <v>9</v>
+      </c>
+      <c r="R24" s="12">
+        <v>1</v>
+      </c>
+      <c r="S24" s="11">
+        <v>2.2E-16</v>
+      </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>3</v>
       </c>
@@ -32208,8 +32267,36 @@
       <c r="G25">
         <v>1.6360496</v>
       </c>
+      <c r="I25">
+        <v>2</v>
+      </c>
+      <c r="J25">
+        <v>2.5505554074535102</v>
+      </c>
+      <c r="K25">
+        <v>2.5477398997380298</v>
+      </c>
+      <c r="M25" t="s">
+        <v>10</v>
+      </c>
+      <c r="N25" s="10">
+        <v>34.344999999999999</v>
+      </c>
+      <c r="O25" s="10">
+        <v>0</v>
+      </c>
+      <c r="P25" s="10"/>
+      <c r="Q25" t="s">
+        <v>10</v>
+      </c>
+      <c r="R25" s="4">
+        <v>2.2E-16</v>
+      </c>
+      <c r="S25" s="13">
+        <v>1</v>
+      </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>3.25</v>
       </c>
@@ -32228,8 +32315,17 @@
       <c r="G26">
         <v>1.2315502</v>
       </c>
+      <c r="I26">
+        <v>3</v>
+      </c>
+      <c r="J26">
+        <v>2.54535181894718</v>
+      </c>
+      <c r="K26">
+        <v>2.5435855958671199</v>
+      </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>3.5</v>
       </c>
@@ -32248,8 +32344,18 @@
       <c r="G27">
         <v>7.6028250000000006E-2</v>
       </c>
+      <c r="I27">
+        <v>4</v>
+      </c>
+      <c r="J27">
+        <v>2.53772691465291</v>
+      </c>
+      <c r="K27">
+        <v>2.5365997228625901</v>
+      </c>
+      <c r="S27" s="11"/>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>3.75</v>
       </c>
@@ -32268,8 +32374,17 @@
       <c r="G28">
         <v>0.58766320000000005</v>
       </c>
+      <c r="I28">
+        <v>5</v>
+      </c>
+      <c r="J28">
+        <v>2.4147228736378299</v>
+      </c>
+      <c r="K28">
+        <v>2.41243006221181</v>
+      </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>4</v>
       </c>
@@ -32288,8 +32403,17 @@
       <c r="G29">
         <v>0.93594940000000004</v>
       </c>
+      <c r="I29">
+        <v>6</v>
+      </c>
+      <c r="J29">
+        <v>1.96151016800439</v>
+      </c>
+      <c r="K29">
+        <v>1.95793523173706</v>
+      </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>4.25</v>
       </c>
@@ -32308,8 +32432,17 @@
       <c r="G30">
         <v>0.58148040000000001</v>
       </c>
+      <c r="I30">
+        <v>7</v>
+      </c>
+      <c r="J30">
+        <v>1.7732462906823001</v>
+      </c>
+      <c r="K30">
+        <v>1.29528035083191</v>
+      </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>4.5</v>
       </c>
@@ -32328,8 +32461,17 @@
       <c r="G31">
         <v>0.13812168</v>
       </c>
+      <c r="I31">
+        <v>8</v>
+      </c>
+      <c r="J31">
+        <v>0.79472344642503601</v>
+      </c>
+      <c r="K31">
+        <v>1.0433824938435201</v>
+      </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>4.75</v>
       </c>
@@ -32348,8 +32490,17 @@
       <c r="G32">
         <v>0.57747256999999996</v>
       </c>
+      <c r="I32">
+        <v>9</v>
+      </c>
+      <c r="J32">
+        <v>0.58968796710425198</v>
+      </c>
+      <c r="K32">
+        <v>0.47560677346927099</v>
+      </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>5</v>
       </c>
@@ -32368,8 +32519,17 @@
       <c r="G33">
         <v>0.91838359999999997</v>
       </c>
+      <c r="I33">
+        <v>10</v>
+      </c>
+      <c r="J33">
+        <v>0.28199545057006897</v>
+      </c>
+      <c r="K33">
+        <v>0.18171930852090701</v>
+      </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>5.25</v>
       </c>
@@ -32389,7 +32549,7 @@
         <v>1.3040259000000001</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>5.5</v>
       </c>
@@ -32408,8 +32568,35 @@
       <c r="G35">
         <v>0.92739930000000004</v>
       </c>
+      <c r="I35" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="J35" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="K35" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="M35" t="s">
+        <v>23</v>
+      </c>
+      <c r="N35" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="O35" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q35" t="s">
+        <v>24</v>
+      </c>
+      <c r="R35" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="S35" s="6" t="s">
+        <v>1</v>
+      </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>5.75</v>
       </c>
@@ -32428,8 +32615,35 @@
       <c r="G36">
         <v>7.5931299999999993E-2</v>
       </c>
+      <c r="I36">
+        <v>1</v>
+      </c>
+      <c r="J36">
+        <v>2.5532883846338899</v>
+      </c>
+      <c r="K36">
+        <v>2.5529877249322501</v>
+      </c>
+      <c r="M36" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="N36" s="10">
+        <v>0</v>
+      </c>
+      <c r="O36" s="10">
+        <v>16.747</v>
+      </c>
+      <c r="Q36" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="R36" s="12">
+        <v>1</v>
+      </c>
+      <c r="S36" s="11">
+        <v>3.629E-5</v>
+      </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>6</v>
       </c>
@@ -32448,8 +32662,36 @@
       <c r="G37">
         <v>0.604688</v>
       </c>
+      <c r="I37">
+        <v>2</v>
+      </c>
+      <c r="J37">
+        <v>2.5505554074535102</v>
+      </c>
+      <c r="K37">
+        <v>2.5477398997380298</v>
+      </c>
+      <c r="M37" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="N37" s="10">
+        <v>16.747</v>
+      </c>
+      <c r="O37" s="10">
+        <v>0</v>
+      </c>
+      <c r="P37" s="10"/>
+      <c r="Q37" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="R37" s="11">
+        <v>3.629E-5</v>
+      </c>
+      <c r="S37" s="13">
+        <v>1</v>
+      </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>6.25</v>
       </c>
@@ -32468,8 +32710,17 @@
       <c r="G38">
         <v>0.96987840000000003</v>
       </c>
+      <c r="I38">
+        <v>3</v>
+      </c>
+      <c r="J38">
+        <v>2.54535181894718</v>
+      </c>
+      <c r="K38">
+        <v>2.5435855958671199</v>
+      </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>6.5</v>
       </c>
@@ -32488,8 +32739,17 @@
       <c r="G39">
         <v>1.4862272999999999</v>
       </c>
+      <c r="I39">
+        <v>4</v>
+      </c>
+      <c r="J39">
+        <v>2.53772691465291</v>
+      </c>
+      <c r="K39">
+        <v>2.5365997228625901</v>
+      </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>6.75</v>
       </c>
@@ -32508,8 +32768,17 @@
       <c r="G40">
         <v>0.62237699999999996</v>
       </c>
+      <c r="I40">
+        <v>5</v>
+      </c>
+      <c r="J40">
+        <v>2.4147228736378299</v>
+      </c>
+      <c r="K40">
+        <v>2.41243006221181</v>
+      </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>7</v>
       </c>
@@ -32528,8 +32797,17 @@
       <c r="G41">
         <v>0.21310903</v>
       </c>
+      <c r="I41">
+        <v>6</v>
+      </c>
+      <c r="J41">
+        <v>1.96151016800439</v>
+      </c>
+      <c r="K41">
+        <v>1.95793523173706</v>
+      </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>7.25</v>
       </c>
@@ -32548,8 +32826,17 @@
       <c r="G42">
         <v>0.63940960000000002</v>
       </c>
+      <c r="I42">
+        <v>7</v>
+      </c>
+      <c r="J42">
+        <v>1.7291236438909099</v>
+      </c>
+      <c r="K42">
+        <v>1.3386346607770601</v>
+      </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>7.5</v>
       </c>
@@ -32568,8 +32855,17 @@
       <c r="G43">
         <v>1.0829565999999999</v>
       </c>
+      <c r="I43">
+        <v>8</v>
+      </c>
+      <c r="J43">
+        <v>1.0736310372529201</v>
+      </c>
+      <c r="K43">
+        <v>1.0414586716202101</v>
+      </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>7.75</v>
       </c>
@@ -32588,8 +32884,17 @@
       <c r="G44">
         <v>1.3043115999999999</v>
       </c>
+      <c r="I44">
+        <v>9</v>
+      </c>
+      <c r="J44">
+        <v>0.59936217387988899</v>
+      </c>
+      <c r="K44">
+        <v>0.51741004930856604</v>
+      </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>8</v>
       </c>
@@ -32608,8 +32913,17 @@
       <c r="G45">
         <v>0.93027203999999997</v>
       </c>
+      <c r="I45">
+        <v>10</v>
+      </c>
+      <c r="J45">
+        <v>0.29911634894509698</v>
+      </c>
+      <c r="K45">
+        <v>0.233693339719897</v>
+      </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>8.25</v>
       </c>
@@ -32629,7 +32943,7 @@
         <v>0.92098146999999997</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>8.5</v>
       </c>
@@ -32648,8 +32962,35 @@
       <c r="G47">
         <v>0.95180900000000002</v>
       </c>
+      <c r="I47" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="J47" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="K47" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="M47" t="s">
+        <v>23</v>
+      </c>
+      <c r="N47" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="O47" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q47" t="s">
+        <v>24</v>
+      </c>
+      <c r="R47" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="S47" s="6" t="s">
+        <v>17</v>
+      </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>8.75</v>
       </c>
@@ -32668,8 +33009,35 @@
       <c r="G48">
         <v>0.9494937</v>
       </c>
+      <c r="I48">
+        <v>1</v>
+      </c>
+      <c r="J48">
+        <v>2.40772858268712</v>
+      </c>
+      <c r="K48">
+        <v>2.4074556325173799</v>
+      </c>
+      <c r="M48" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="N48" s="10">
+        <v>0</v>
+      </c>
+      <c r="O48" s="10">
+        <v>16.149999999999999</v>
+      </c>
+      <c r="Q48" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="R48" s="12">
+        <v>1</v>
+      </c>
+      <c r="S48" s="10">
+        <v>8.7319999999999997E-5</v>
+      </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>9</v>
       </c>
@@ -32688,8 +33056,36 @@
       <c r="G49">
         <v>0.97163193999999997</v>
       </c>
+      <c r="I49">
+        <v>2</v>
+      </c>
+      <c r="J49">
+        <v>2.40382888512034</v>
+      </c>
+      <c r="K49">
+        <v>2.4014276030405299</v>
+      </c>
+      <c r="M49" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="N49" s="10">
+        <v>16.149999999999999</v>
+      </c>
+      <c r="O49" s="10">
+        <v>0</v>
+      </c>
+      <c r="P49" s="10"/>
+      <c r="Q49" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="R49" s="10">
+        <v>8.7319999999999997E-5</v>
+      </c>
+      <c r="S49" s="13">
+        <v>1</v>
+      </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>9.25</v>
       </c>
@@ -32708,8 +33104,17 @@
       <c r="G50">
         <v>0.80045825000000004</v>
       </c>
+      <c r="I50">
+        <v>3</v>
+      </c>
+      <c r="J50" s="4">
+        <v>2.4010104043791101</v>
+      </c>
+      <c r="K50">
+        <v>2.3948106423125899</v>
+      </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>9.5</v>
       </c>
@@ -32728,8 +33133,17 @@
       <c r="G51">
         <v>0.66504399999999997</v>
       </c>
+      <c r="I51">
+        <v>4</v>
+      </c>
+      <c r="J51">
+        <v>2.3961440432977499</v>
+      </c>
+      <c r="K51">
+        <v>2.3876217050610999</v>
+      </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>9.75</v>
       </c>
@@ -32747,6 +33161,246 @@
       </c>
       <c r="G52">
         <v>0.74505560000000004</v>
+      </c>
+      <c r="I52">
+        <v>5</v>
+      </c>
+      <c r="J52">
+        <v>2.3386448247934299</v>
+      </c>
+      <c r="K52">
+        <v>2.3380419708430802</v>
+      </c>
+    </row>
+    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="I53">
+        <v>6</v>
+      </c>
+      <c r="J53">
+        <v>1.9716103621054999</v>
+      </c>
+      <c r="K53">
+        <v>1.8617380009025699</v>
+      </c>
+    </row>
+    <row r="54" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="I54">
+        <v>7</v>
+      </c>
+      <c r="J54">
+        <v>1.5097331919243699</v>
+      </c>
+      <c r="K54">
+        <v>1.4040843303577799</v>
+      </c>
+    </row>
+    <row r="55" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="I55">
+        <v>8</v>
+      </c>
+      <c r="J55">
+        <v>1.0685105775080499</v>
+      </c>
+      <c r="K55">
+        <v>0.90412141379983901</v>
+      </c>
+    </row>
+    <row r="56" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="I56">
+        <v>9</v>
+      </c>
+      <c r="J56">
+        <v>0.625007323845163</v>
+      </c>
+      <c r="K56">
+        <v>0.55883012125238096</v>
+      </c>
+    </row>
+    <row r="57" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="I57">
+        <v>10</v>
+      </c>
+      <c r="J57">
+        <v>0.415025755405944</v>
+      </c>
+      <c r="K57">
+        <v>0.28542641071339803</v>
+      </c>
+    </row>
+    <row r="59" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="I59" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="J59" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="K59" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="M59" t="s">
+        <v>23</v>
+      </c>
+      <c r="N59" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="O59" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q59" t="s">
+        <v>24</v>
+      </c>
+      <c r="R59" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="S59" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="60" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="I60">
+        <v>1</v>
+      </c>
+      <c r="J60">
+        <v>2.5532883846338899</v>
+      </c>
+      <c r="K60">
+        <v>2.5529877249322501</v>
+      </c>
+      <c r="M60" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="N60" s="10">
+        <v>0</v>
+      </c>
+      <c r="O60" s="10">
+        <v>17.963999999999999</v>
+      </c>
+      <c r="Q60" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="R60" s="12">
+        <v>1</v>
+      </c>
+      <c r="S60" s="10">
+        <v>1.48858E-4</v>
+      </c>
+    </row>
+    <row r="61" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="I61">
+        <v>2</v>
+      </c>
+      <c r="J61">
+        <v>2.5505554074535102</v>
+      </c>
+      <c r="K61">
+        <v>2.5477398997380298</v>
+      </c>
+      <c r="M61" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="N61" s="10">
+        <v>17.963999999999999</v>
+      </c>
+      <c r="O61" s="10">
+        <v>0</v>
+      </c>
+      <c r="P61" s="10"/>
+      <c r="Q61" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="R61" s="10">
+        <v>1.48858E-4</v>
+      </c>
+      <c r="S61" s="13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="62" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="I62">
+        <v>3</v>
+      </c>
+      <c r="J62">
+        <v>2.54535181894718</v>
+      </c>
+      <c r="K62">
+        <v>2.5435855958671199</v>
+      </c>
+    </row>
+    <row r="63" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="I63">
+        <v>4</v>
+      </c>
+      <c r="J63">
+        <v>2.53772691465291</v>
+      </c>
+      <c r="K63">
+        <v>2.5365997228625901</v>
+      </c>
+    </row>
+    <row r="64" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="I64">
+        <v>5</v>
+      </c>
+      <c r="J64">
+        <v>2.4147228736378299</v>
+      </c>
+      <c r="K64">
+        <v>2.41243006221181</v>
+      </c>
+    </row>
+    <row r="65" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I65">
+        <v>6</v>
+      </c>
+      <c r="J65">
+        <v>1.96151016800439</v>
+      </c>
+      <c r="K65">
+        <v>1.95793523173706</v>
+      </c>
+    </row>
+    <row r="66" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I66">
+        <v>7</v>
+      </c>
+      <c r="J66">
+        <v>1.7291236438909099</v>
+      </c>
+      <c r="K66">
+        <v>1.3386346607770601</v>
+      </c>
+    </row>
+    <row r="67" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I67">
+        <v>8</v>
+      </c>
+      <c r="J67">
+        <v>1.0736310372529201</v>
+      </c>
+      <c r="K67">
+        <v>1.0414586716202101</v>
+      </c>
+    </row>
+    <row r="68" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I68">
+        <v>9</v>
+      </c>
+      <c r="J68">
+        <v>0.59936217387988899</v>
+      </c>
+      <c r="K68">
+        <v>0.51741004930856604</v>
+      </c>
+    </row>
+    <row r="69" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I69">
+        <v>10</v>
+      </c>
+      <c r="J69">
+        <v>0.29911634894509698</v>
+      </c>
+      <c r="K69">
+        <v>0.233693339719897</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
exp2 report, exp2 t-test
</commit_message>
<xml_diff>
--- a/Project_3/data.xlsx
+++ b/Project_3/data.xlsx
@@ -96,7 +96,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -147,12 +147,6 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Lucida Console"/>
-      <family val="3"/>
-    </font>
   </fonts>
   <fills count="7">
     <fill>
@@ -187,7 +181,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -225,6 +219,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -234,7 +243,7 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="6" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
@@ -247,16 +256,7 @@
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="11" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="1" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Calculation" xfId="4" builtinId="22"/>
@@ -27711,8 +27711,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AJ100"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="A62" sqref="A62:K64"/>
+    <sheetView topLeftCell="B56" workbookViewId="0">
+      <selection activeCell="B73" sqref="B73:K73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -31559,99 +31559,101 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="S66" sqref="S66"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="Q59" sqref="Q59:S61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="11" max="12" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="17" width="10.140625" bestFit="1" customWidth="1"/>
-    <col min="18" max="19" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="10" width="9.140625" style="10"/>
+    <col min="11" max="12" width="10.140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.140625" style="10"/>
+    <col min="14" max="17" width="10.140625" style="10" bestFit="1" customWidth="1"/>
+    <col min="18" max="19" width="12.42578125" style="10" bestFit="1" customWidth="1"/>
+    <col min="20" max="16384" width="9.140625" style="10"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A1" s="3"/>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="10" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="A2" s="10">
         <v>1</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="10">
         <v>2.5365204029999999</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="10">
         <v>2.205841924</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="10">
         <v>2.7523920070000001</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="10">
         <v>2.4167213649999999</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="I2" t="s">
+      <c r="I2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="K2" t="s">
+      <c r="K2" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="M2" t="s">
+      <c r="M2" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="N2" s="1" t="s">
+      <c r="N2" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="O2" t="s">
+      <c r="O2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="P2" t="s">
+      <c r="P2" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="Q2" s="10" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="A3" s="10">
         <v>2</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="10">
         <v>2.622415937</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="10">
         <v>2.406436121</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="10">
         <v>2.6584313900000001</v>
       </c>
-      <c r="E3">
+      <c r="E3" s="10">
         <v>2.4122123329999998</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="G3" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="10">
         <v>0</v>
       </c>
       <c r="I3" s="10">
@@ -31663,17 +31665,16 @@
       <c r="K3" s="10">
         <v>5.9733999999999998</v>
       </c>
-      <c r="L3" s="10"/>
-      <c r="M3" s="1" t="s">
+      <c r="M3" s="10" t="s">
         <v>0</v>
       </c>
-      <c r="N3">
+      <c r="N3" s="10">
         <v>1</v>
       </c>
-      <c r="O3" s="11">
+      <c r="O3" s="10">
         <v>1.265E-7</v>
       </c>
-      <c r="P3" s="11">
+      <c r="P3" s="10">
         <v>3.629E-5</v>
       </c>
       <c r="Q3" s="10">
@@ -31681,28 +31682,28 @@
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="A4" s="10">
         <v>3</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="10">
         <v>2.4586656069999999</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="10">
         <v>2.3019097660000001</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="10">
         <v>2.6924265169999999</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="10">
         <v>2.4168705209999999</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G4" s="10" t="s">
         <v>1</v>
       </c>
       <c r="H4" s="10">
         <v>8.4078999999999997</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="10">
         <v>0</v>
       </c>
       <c r="J4" s="10">
@@ -31711,16 +31712,16 @@
       <c r="K4" s="10">
         <v>5.9188000000000001</v>
       </c>
-      <c r="M4" t="s">
+      <c r="M4" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="N4" s="11">
+      <c r="N4" s="10">
         <v>1.265E-7</v>
       </c>
-      <c r="O4">
+      <c r="O4" s="10">
         <v>1</v>
       </c>
-      <c r="P4" s="11">
+      <c r="P4" s="10">
         <v>3.328E-11</v>
       </c>
       <c r="Q4" s="10">
@@ -31728,22 +31729,22 @@
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="A5" s="10">
         <v>4</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="10">
         <v>2.6340233400000002</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="10">
         <v>2.2289593829999998</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="10">
         <v>2.7489202079999999</v>
       </c>
-      <c r="E5">
+      <c r="E5" s="10">
         <v>2.4166907119999999</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" s="10" t="s">
         <v>11</v>
       </c>
       <c r="H5" s="10">
@@ -31752,45 +31753,45 @@
       <c r="I5" s="10">
         <v>16.747</v>
       </c>
-      <c r="J5">
+      <c r="J5" s="10">
         <v>0</v>
       </c>
       <c r="K5" s="10">
         <v>21.954999999999998</v>
       </c>
-      <c r="M5" t="s">
+      <c r="M5" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="N5" s="11">
+      <c r="N5" s="10">
         <v>3.629E-5</v>
       </c>
-      <c r="O5" s="11">
+      <c r="O5" s="10">
         <v>3.328E-11</v>
       </c>
-      <c r="P5">
+      <c r="P5" s="10">
         <v>1</v>
       </c>
-      <c r="Q5" s="11">
+      <c r="Q5" s="10">
         <v>3.6560000000000002E-9</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="A6" s="10">
         <v>5</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="10">
         <v>2.4361303539999999</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="10">
         <v>2.2498002559999999</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="10">
         <v>2.6839354879999999</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="10">
         <v>2.4183203199999999</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G6" s="10" t="s">
         <v>3</v>
       </c>
       <c r="H6" s="10">
@@ -31802,140 +31803,140 @@
       <c r="J6" s="10">
         <v>21.954999999999998</v>
       </c>
-      <c r="K6">
+      <c r="K6" s="10">
         <v>0</v>
       </c>
-      <c r="M6" t="s">
+      <c r="M6" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="N6" s="11">
+      <c r="N6" s="10">
         <v>9.2879999999999995E-8</v>
       </c>
       <c r="O6" s="10">
         <v>2.2169999999999999E-4</v>
       </c>
-      <c r="P6" s="11">
+      <c r="P6" s="10">
         <v>3.6560000000000002E-9</v>
       </c>
-      <c r="Q6">
+      <c r="Q6" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A7">
+      <c r="A7" s="10">
         <v>6</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="10">
         <v>2.5916865260000002</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="10">
         <v>2.2961825820000001</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="10">
         <v>2.640776206</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="10">
         <v>2.4119548040000001</v>
       </c>
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A8">
+      <c r="A8" s="10">
         <v>7</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="10">
         <v>2.6327983850000001</v>
       </c>
-      <c r="C8">
+      <c r="C8" s="10">
         <v>2.3345638379999998</v>
       </c>
-      <c r="D8">
+      <c r="D8" s="10">
         <v>2.7440153139999999</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="10">
         <v>2.413074881</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A9">
+      <c r="A9" s="10">
         <v>8</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="10">
         <v>2.6173958050000001</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="10">
         <v>2.2424187369999999</v>
       </c>
-      <c r="D9">
+      <c r="D9" s="10">
         <v>2.7300926689999998</v>
       </c>
-      <c r="E9">
+      <c r="E9" s="10">
         <v>2.4137620279999998</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A10">
+      <c r="A10" s="10">
         <v>9</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="10">
         <v>2.5055857700000002</v>
       </c>
-      <c r="C10">
+      <c r="C10" s="10">
         <v>2.3774054069999999</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="10">
         <v>2.767659664</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="10">
         <v>2.4166710899999999</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A11">
+      <c r="A11" s="10">
         <v>10</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="10">
         <v>2.5176663079999999</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="10">
         <v>2.2269797470000001</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="10">
         <v>2.7269301279999998</v>
       </c>
-      <c r="E11">
+      <c r="E11" s="10">
         <v>2.4126289010000002</v>
       </c>
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="I12" t="s">
+      <c r="I12" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="M12" t="s">
+      <c r="M12" s="10" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="I13" t="s">
+      <c r="I13" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="J13" t="s">
+      <c r="J13" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="K13" t="s">
+      <c r="K13" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="M13" t="s">
+      <c r="M13" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="N13" t="s">
+      <c r="N13" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="O13" t="s">
+      <c r="O13" s="10" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="I14" t="s">
+      <c r="I14" s="10" t="s">
         <v>18</v>
       </c>
       <c r="J14" s="10">
@@ -31944,18 +31945,18 @@
       <c r="K14" s="10">
         <v>7.1547000000000001</v>
       </c>
-      <c r="M14" t="s">
+      <c r="M14" s="10" t="s">
         <v>18</v>
       </c>
       <c r="N14" s="10">
         <v>1</v>
       </c>
-      <c r="O14" s="11">
+      <c r="O14" s="10">
         <v>1.564E-9</v>
       </c>
     </row>
     <row r="15" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="I15" t="s">
+      <c r="I15" s="10" t="s">
         <v>19</v>
       </c>
       <c r="J15" s="10">
@@ -31964,10 +31965,10 @@
       <c r="K15" s="10">
         <v>0</v>
       </c>
-      <c r="M15" t="s">
+      <c r="M15" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="N15" s="11">
+      <c r="N15" s="10">
         <v>1.564E-9</v>
       </c>
       <c r="O15" s="10">
@@ -31975,89 +31976,89 @@
       </c>
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
+      <c r="A17" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B17" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="E17" s="3" t="s">
+      <c r="E17" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F17" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="G17" t="s">
+      <c r="G17" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="I17" t="s">
+      <c r="I17" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="M17" t="s">
+      <c r="M17" s="10" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A18">
+      <c r="A18" s="10">
         <v>1.25</v>
       </c>
-      <c r="B18" s="9">
+      <c r="B18" s="10">
         <v>1.7990558999999999</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="10">
         <v>0.88161235999999998</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="10">
         <v>1.25</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="10">
         <v>1.9642427</v>
       </c>
-      <c r="G18">
+      <c r="G18" s="10">
         <v>0.86211055999999997</v>
       </c>
-      <c r="I18" t="s">
+      <c r="I18" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="J18" t="s">
+      <c r="J18" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="K18" t="s">
+      <c r="K18" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="M18" t="s">
+      <c r="M18" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="N18" t="s">
+      <c r="N18" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="O18" t="s">
+      <c r="O18" s="10" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A19">
+      <c r="A19" s="10">
         <v>1.5</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="10">
         <v>1.9661234999999999</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="10">
         <v>0.91965350000000001</v>
       </c>
-      <c r="E19">
+      <c r="E19" s="10">
         <v>1.5</v>
       </c>
-      <c r="F19">
+      <c r="F19" s="10">
         <v>1.8559382</v>
       </c>
-      <c r="G19">
+      <c r="G19" s="10">
         <v>1.2555703</v>
       </c>
-      <c r="I19" t="s">
+      <c r="I19" s="10" t="s">
         <v>18</v>
       </c>
       <c r="J19" s="10">
@@ -32066,36 +32067,36 @@
       <c r="K19" s="10">
         <v>8.0890000000000004</v>
       </c>
-      <c r="M19" t="s">
+      <c r="M19" s="10" t="s">
         <v>18</v>
       </c>
       <c r="N19" s="10">
         <v>1</v>
       </c>
-      <c r="O19" s="11">
+      <c r="O19" s="10">
         <v>1.8419999999999999E-11</v>
       </c>
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A20">
+      <c r="A20" s="10">
         <v>1.75</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="10">
         <v>1.9286816</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="10">
         <v>0.92048054999999995</v>
       </c>
-      <c r="E20">
+      <c r="E20" s="10">
         <v>1.75</v>
       </c>
-      <c r="F20">
+      <c r="F20" s="10">
         <v>1.8436201000000001</v>
       </c>
-      <c r="G20">
+      <c r="G20" s="10">
         <v>1.7207104</v>
       </c>
-      <c r="I20" t="s">
+      <c r="I20" s="10" t="s">
         <v>19</v>
       </c>
       <c r="J20" s="10">
@@ -32104,10 +32105,10 @@
       <c r="K20" s="10">
         <v>0</v>
       </c>
-      <c r="M20" t="s">
+      <c r="M20" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="N20" s="11">
+      <c r="N20" s="10">
         <v>1.8419999999999999E-11</v>
       </c>
       <c r="O20" s="10">
@@ -32115,121 +32116,121 @@
       </c>
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A21">
+      <c r="A21" s="10">
         <v>2</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="10">
         <v>1.9129444</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="10">
         <v>0.75735724000000004</v>
       </c>
-      <c r="E21">
+      <c r="E21" s="10">
         <v>2</v>
       </c>
-      <c r="F21">
+      <c r="F21" s="10">
         <v>1.8959904999999999</v>
       </c>
-      <c r="G21">
+      <c r="G21" s="10">
         <v>0.64572143999999998</v>
       </c>
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A22">
+      <c r="A22" s="10">
         <v>2.25</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="10">
         <v>1.8592785999999999</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="10">
         <v>1.0361407</v>
       </c>
-      <c r="E22">
+      <c r="E22" s="10">
         <v>2.25</v>
       </c>
-      <c r="F22">
+      <c r="F22" s="10">
         <v>1.9610088999999999</v>
       </c>
-      <c r="G22">
+      <c r="G22" s="10">
         <v>0.19783816000000001</v>
       </c>
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A23">
+      <c r="A23" s="10">
         <v>2.5</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="10">
         <v>1.8494748000000001</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="10">
         <v>1.4915395</v>
       </c>
-      <c r="E23">
+      <c r="E23" s="10">
         <v>2.5</v>
       </c>
-      <c r="F23">
+      <c r="F23" s="10">
         <v>1.963544</v>
       </c>
-      <c r="G23">
+      <c r="G23" s="10">
         <v>0.68800455000000005</v>
       </c>
-      <c r="I23" t="s">
+      <c r="I23" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="J23" t="s">
+      <c r="J23" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="K23" t="s">
+      <c r="K23" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="M23" t="s">
+      <c r="M23" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="N23" t="s">
+      <c r="N23" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="O23" t="s">
+      <c r="O23" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="Q23" t="s">
+      <c r="Q23" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="R23" t="s">
+      <c r="R23" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="S23" t="s">
+      <c r="S23" s="10" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A24">
+      <c r="A24" s="10">
         <v>2.75</v>
       </c>
-      <c r="B24">
+      <c r="B24" s="10">
         <v>1.8959904999999999</v>
       </c>
-      <c r="C24">
+      <c r="C24" s="10">
         <v>1.1375299000000001</v>
       </c>
-      <c r="E24">
+      <c r="E24" s="10">
         <v>2.75</v>
       </c>
-      <c r="F24">
+      <c r="F24" s="10">
         <v>1.9626402999999999</v>
       </c>
-      <c r="G24">
+      <c r="G24" s="10">
         <v>1.0750082999999999</v>
       </c>
-      <c r="I24">
+      <c r="I24" s="10">
         <v>1</v>
       </c>
-      <c r="J24">
+      <c r="J24" s="10">
         <v>2.5532883846338899</v>
       </c>
-      <c r="K24">
+      <c r="K24" s="10">
         <v>2.5529877249322501</v>
       </c>
-      <c r="M24" t="s">
+      <c r="M24" s="10" t="s">
         <v>9</v>
       </c>
       <c r="N24" s="10">
@@ -32238,45 +32239,45 @@
       <c r="O24" s="10">
         <v>34.344999999999999</v>
       </c>
-      <c r="Q24" t="s">
+      <c r="Q24" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="R24" s="12">
+      <c r="R24" s="10">
         <v>1</v>
       </c>
-      <c r="S24" s="11">
+      <c r="S24" s="10">
         <v>2.2E-16</v>
       </c>
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A25">
+      <c r="A25" s="10">
         <v>3</v>
       </c>
-      <c r="B25">
+      <c r="B25" s="10">
         <v>1.9597555</v>
       </c>
-      <c r="C25">
+      <c r="C25" s="10">
         <v>1.1646798</v>
       </c>
-      <c r="E25">
+      <c r="E25" s="10">
         <v>3</v>
       </c>
-      <c r="F25">
+      <c r="F25" s="10">
         <v>1.9560598</v>
       </c>
-      <c r="G25">
+      <c r="G25" s="10">
         <v>1.6360496</v>
       </c>
-      <c r="I25">
+      <c r="I25" s="10">
         <v>2</v>
       </c>
-      <c r="J25">
+      <c r="J25" s="10">
         <v>2.5505554074535102</v>
       </c>
-      <c r="K25">
+      <c r="K25" s="10">
         <v>2.5477398997380298</v>
       </c>
-      <c r="M25" t="s">
+      <c r="M25" s="10" t="s">
         <v>10</v>
       </c>
       <c r="N25" s="10">
@@ -32285,346 +32286,344 @@
       <c r="O25" s="10">
         <v>0</v>
       </c>
-      <c r="P25" s="10"/>
-      <c r="Q25" t="s">
+      <c r="Q25" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="R25" s="4">
+      <c r="R25" s="10">
         <v>2.2E-16</v>
       </c>
-      <c r="S25" s="13">
+      <c r="S25" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A26">
+      <c r="A26" s="10">
         <v>3.25</v>
       </c>
-      <c r="B26">
+      <c r="B26" s="10">
         <v>1.9648021</v>
       </c>
-      <c r="C26">
+      <c r="C26" s="10">
         <v>0.85121422999999996</v>
       </c>
-      <c r="E26">
+      <c r="E26" s="10">
         <v>3.25</v>
       </c>
-      <c r="F26">
+      <c r="F26" s="10">
         <v>1.9380782999999999</v>
       </c>
-      <c r="G26">
+      <c r="G26" s="10">
         <v>1.2315502</v>
       </c>
-      <c r="I26">
+      <c r="I26" s="10">
         <v>3</v>
       </c>
-      <c r="J26">
+      <c r="J26" s="10">
         <v>2.54535181894718</v>
       </c>
-      <c r="K26">
+      <c r="K26" s="10">
         <v>2.5435855958671199</v>
       </c>
     </row>
     <row r="27" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A27">
+      <c r="A27" s="10">
         <v>3.5</v>
       </c>
-      <c r="B27">
+      <c r="B27" s="10">
         <v>1.9626402999999999</v>
       </c>
-      <c r="C27">
+      <c r="C27" s="10">
         <v>1.0996870000000001</v>
       </c>
-      <c r="E27">
+      <c r="E27" s="10">
         <v>3.5</v>
       </c>
-      <c r="F27">
+      <c r="F27" s="10">
         <v>1.9478873999999999</v>
       </c>
-      <c r="G27">
+      <c r="G27" s="10">
         <v>7.6028250000000006E-2</v>
       </c>
-      <c r="I27">
+      <c r="I27" s="10">
         <v>4</v>
       </c>
-      <c r="J27">
+      <c r="J27" s="10">
         <v>2.53772691465291</v>
       </c>
-      <c r="K27">
+      <c r="K27" s="10">
         <v>2.5365997228625901</v>
       </c>
-      <c r="S27" s="11"/>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A28">
+      <c r="A28" s="10">
         <v>3.75</v>
       </c>
-      <c r="B28">
+      <c r="B28" s="10">
         <v>1.9560598</v>
       </c>
-      <c r="C28">
+      <c r="C28" s="10">
         <v>1.6315086000000001</v>
       </c>
-      <c r="E28">
+      <c r="E28" s="10">
         <v>3.75</v>
       </c>
-      <c r="F28">
+      <c r="F28" s="10">
         <v>1.9799609</v>
       </c>
-      <c r="G28">
+      <c r="G28" s="10">
         <v>0.58766320000000005</v>
       </c>
-      <c r="I28">
+      <c r="I28" s="10">
         <v>5</v>
       </c>
-      <c r="J28">
+      <c r="J28" s="10">
         <v>2.4147228736378299</v>
       </c>
-      <c r="K28">
+      <c r="K28" s="10">
         <v>2.41243006221181</v>
       </c>
     </row>
     <row r="29" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A29">
+      <c r="A29" s="10">
         <v>4</v>
       </c>
-      <c r="B29">
+      <c r="B29" s="10">
         <v>1.9380782999999999</v>
       </c>
-      <c r="C29">
+      <c r="C29" s="10">
         <v>1.1773625999999999</v>
       </c>
-      <c r="E29">
+      <c r="E29" s="10">
         <v>4</v>
       </c>
-      <c r="F29">
+      <c r="F29" s="10">
         <v>1.9317724999999999</v>
       </c>
-      <c r="G29">
+      <c r="G29" s="10">
         <v>0.93594940000000004</v>
       </c>
-      <c r="I29">
+      <c r="I29" s="10">
         <v>6</v>
       </c>
-      <c r="J29">
+      <c r="J29" s="10">
         <v>1.96151016800439</v>
       </c>
-      <c r="K29">
+      <c r="K29" s="10">
         <v>1.95793523173706</v>
       </c>
     </row>
     <row r="30" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A30">
+      <c r="A30" s="10">
         <v>4.25</v>
       </c>
-      <c r="B30">
+      <c r="B30" s="10">
         <v>1.9478873999999999</v>
       </c>
-      <c r="C30">
+      <c r="C30" s="10">
         <v>1.0909137</v>
       </c>
-      <c r="E30">
+      <c r="E30" s="10">
         <v>4.25</v>
       </c>
-      <c r="F30">
+      <c r="F30" s="10">
         <v>1.9255310999999999</v>
       </c>
-      <c r="G30">
+      <c r="G30" s="10">
         <v>0.58148040000000001</v>
       </c>
-      <c r="I30">
+      <c r="I30" s="10">
         <v>7</v>
       </c>
-      <c r="J30">
+      <c r="J30" s="10">
         <v>1.7732462906823001</v>
       </c>
-      <c r="K30">
+      <c r="K30" s="10">
         <v>1.29528035083191</v>
       </c>
     </row>
     <row r="31" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A31">
+      <c r="A31" s="10">
         <v>4.5</v>
       </c>
-      <c r="B31">
+      <c r="B31" s="10">
         <v>1.9799609</v>
       </c>
-      <c r="C31">
+      <c r="C31" s="10">
         <v>0.81111752999999998</v>
       </c>
-      <c r="E31">
+      <c r="E31" s="10">
         <v>4.5</v>
       </c>
-      <c r="F31">
+      <c r="F31" s="10">
         <v>1.9457603999999999</v>
       </c>
-      <c r="G31">
+      <c r="G31" s="10">
         <v>0.13812168</v>
       </c>
-      <c r="I31">
+      <c r="I31" s="10">
         <v>8</v>
       </c>
-      <c r="J31">
+      <c r="J31" s="10">
         <v>0.79472344642503601</v>
       </c>
-      <c r="K31">
+      <c r="K31" s="10">
         <v>1.0433824938435201</v>
       </c>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A32">
+      <c r="A32" s="10">
         <v>4.75</v>
       </c>
-      <c r="B32">
+      <c r="B32" s="10">
         <v>1.9317724999999999</v>
       </c>
-      <c r="C32">
+      <c r="C32" s="10">
         <v>1.0376289999999999</v>
       </c>
-      <c r="E32">
+      <c r="E32" s="10">
         <v>4.75</v>
       </c>
-      <c r="F32">
+      <c r="F32" s="10">
         <v>1.9568653</v>
       </c>
-      <c r="G32">
+      <c r="G32" s="10">
         <v>0.57747256999999996</v>
       </c>
-      <c r="I32">
+      <c r="I32" s="10">
         <v>9</v>
       </c>
-      <c r="J32">
+      <c r="J32" s="10">
         <v>0.58968796710425198</v>
       </c>
-      <c r="K32">
+      <c r="K32" s="10">
         <v>0.47560677346927099</v>
       </c>
     </row>
     <row r="33" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A33">
+      <c r="A33" s="10">
         <v>5</v>
       </c>
-      <c r="B33">
+      <c r="B33" s="10">
         <v>1.9255310999999999</v>
       </c>
-      <c r="C33">
+      <c r="C33" s="10">
         <v>0.72743164999999999</v>
       </c>
-      <c r="E33">
+      <c r="E33" s="10">
         <v>5</v>
       </c>
-      <c r="F33">
+      <c r="F33" s="10">
         <v>1.9604653000000001</v>
       </c>
-      <c r="G33">
+      <c r="G33" s="10">
         <v>0.91838359999999997</v>
       </c>
-      <c r="I33">
+      <c r="I33" s="10">
         <v>10</v>
       </c>
-      <c r="J33">
+      <c r="J33" s="10">
         <v>0.28199545057006897</v>
       </c>
-      <c r="K33">
+      <c r="K33" s="10">
         <v>0.18171930852090701</v>
       </c>
     </row>
     <row r="34" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A34">
+      <c r="A34" s="10">
         <v>5.25</v>
       </c>
-      <c r="B34">
+      <c r="B34" s="10">
         <v>1.9457603999999999</v>
       </c>
-      <c r="C34">
+      <c r="C34" s="10">
         <v>1.2585522</v>
       </c>
-      <c r="E34">
+      <c r="E34" s="10">
         <v>5.25</v>
       </c>
-      <c r="F34">
+      <c r="F34" s="10">
         <v>1.9552666000000001</v>
       </c>
-      <c r="G34">
+      <c r="G34" s="10">
         <v>1.3040259000000001</v>
       </c>
     </row>
     <row r="35" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A35">
+      <c r="A35" s="10">
         <v>5.5</v>
       </c>
-      <c r="B35">
+      <c r="B35" s="10">
         <v>1.9568653</v>
       </c>
-      <c r="C35">
+      <c r="C35" s="10">
         <v>1.6249425</v>
       </c>
-      <c r="E35">
+      <c r="E35" s="10">
         <v>5.5</v>
       </c>
-      <c r="F35">
+      <c r="F35" s="10">
         <v>1.8652314000000001</v>
       </c>
-      <c r="G35">
+      <c r="G35" s="10">
         <v>0.92739930000000004</v>
       </c>
-      <c r="I35" s="3" t="s">
+      <c r="I35" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="J35" s="6" t="s">
+      <c r="J35" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="K35" s="6" t="s">
+      <c r="K35" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="M35" t="s">
+      <c r="M35" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="N35" s="6" t="s">
+      <c r="N35" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="O35" s="6" t="s">
+      <c r="O35" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="Q35" t="s">
+      <c r="Q35" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="R35" s="6" t="s">
+      <c r="R35" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="S35" s="6" t="s">
+      <c r="S35" s="10" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A36">
+      <c r="A36" s="10">
         <v>5.75</v>
       </c>
-      <c r="B36">
+      <c r="B36" s="10">
         <v>1.9604653000000001</v>
       </c>
-      <c r="C36">
+      <c r="C36" s="10">
         <v>1.910839</v>
       </c>
-      <c r="E36">
+      <c r="E36" s="10">
         <v>5.75</v>
       </c>
-      <c r="F36">
+      <c r="F36" s="10">
         <v>1.9321562000000001</v>
       </c>
-      <c r="G36">
+      <c r="G36" s="10">
         <v>7.5931299999999993E-2</v>
       </c>
-      <c r="I36">
+      <c r="I36" s="10">
         <v>1</v>
       </c>
-      <c r="J36">
+      <c r="J36" s="10">
         <v>2.5532883846338899</v>
       </c>
-      <c r="K36">
+      <c r="K36" s="10">
         <v>2.5529877249322501</v>
       </c>
-      <c r="M36" s="6" t="s">
+      <c r="M36" s="10" t="s">
         <v>11</v>
       </c>
       <c r="N36" s="10">
@@ -32633,45 +32632,45 @@
       <c r="O36" s="10">
         <v>16.747</v>
       </c>
-      <c r="Q36" s="6" t="s">
+      <c r="Q36" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="R36" s="12">
+      <c r="R36" s="10">
         <v>1</v>
       </c>
-      <c r="S36" s="11">
+      <c r="S36" s="10">
         <v>3.629E-5</v>
       </c>
     </row>
     <row r="37" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A37">
+      <c r="A37" s="10">
         <v>6</v>
       </c>
-      <c r="B37">
+      <c r="B37" s="10">
         <v>1.9552666000000001</v>
       </c>
-      <c r="C37">
+      <c r="C37" s="10">
         <v>1.9190174</v>
       </c>
-      <c r="E37">
+      <c r="E37" s="10">
         <v>6</v>
       </c>
-      <c r="F37">
+      <c r="F37" s="10">
         <v>1.9773959000000001</v>
       </c>
-      <c r="G37">
+      <c r="G37" s="10">
         <v>0.604688</v>
       </c>
-      <c r="I37">
+      <c r="I37" s="10">
         <v>2</v>
       </c>
-      <c r="J37">
+      <c r="J37" s="10">
         <v>2.5505554074535102</v>
       </c>
-      <c r="K37">
+      <c r="K37" s="10">
         <v>2.5477398997380298</v>
       </c>
-      <c r="M37" s="6" t="s">
+      <c r="M37" s="10" t="s">
         <v>1</v>
       </c>
       <c r="N37" s="10">
@@ -32680,345 +32679,344 @@
       <c r="O37" s="10">
         <v>0</v>
       </c>
-      <c r="P37" s="10"/>
-      <c r="Q37" s="6" t="s">
+      <c r="Q37" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="R37" s="11">
+      <c r="R37" s="10">
         <v>3.629E-5</v>
       </c>
-      <c r="S37" s="13">
+      <c r="S37" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A38">
+      <c r="A38" s="10">
         <v>6.25</v>
       </c>
-      <c r="B38">
+      <c r="B38" s="10">
         <v>1.8652314000000001</v>
       </c>
-      <c r="C38">
+      <c r="C38" s="10">
         <v>1.9524615999999999</v>
       </c>
-      <c r="E38">
+      <c r="E38" s="10">
         <v>6.25</v>
       </c>
-      <c r="F38">
+      <c r="F38" s="10">
         <v>1.9696094</v>
       </c>
-      <c r="G38">
+      <c r="G38" s="10">
         <v>0.96987840000000003</v>
       </c>
-      <c r="I38">
+      <c r="I38" s="10">
         <v>3</v>
       </c>
-      <c r="J38">
+      <c r="J38" s="10">
         <v>2.54535181894718</v>
       </c>
-      <c r="K38">
+      <c r="K38" s="10">
         <v>2.5435855958671199</v>
       </c>
     </row>
     <row r="39" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A39">
+      <c r="A39" s="10">
         <v>6.5</v>
       </c>
-      <c r="B39">
+      <c r="B39" s="10">
         <v>1.9321562000000001</v>
       </c>
-      <c r="C39">
+      <c r="C39" s="10">
         <v>1.9450635000000001</v>
       </c>
-      <c r="E39">
+      <c r="E39" s="10">
         <v>6.5</v>
       </c>
-      <c r="F39">
+      <c r="F39" s="10">
         <v>1.7583034</v>
       </c>
-      <c r="G39">
+      <c r="G39" s="10">
         <v>1.4862272999999999</v>
       </c>
-      <c r="I39">
+      <c r="I39" s="10">
         <v>4</v>
       </c>
-      <c r="J39">
+      <c r="J39" s="10">
         <v>2.53772691465291</v>
       </c>
-      <c r="K39">
+      <c r="K39" s="10">
         <v>2.5365997228625901</v>
       </c>
     </row>
     <row r="40" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A40">
+      <c r="A40" s="10">
         <v>6.75</v>
       </c>
-      <c r="B40">
+      <c r="B40" s="10">
         <v>1.9773959000000001</v>
       </c>
-      <c r="C40">
+      <c r="C40" s="10">
         <v>1.9665736</v>
       </c>
-      <c r="E40">
+      <c r="E40" s="10">
         <v>6.75</v>
       </c>
-      <c r="F40">
+      <c r="F40" s="10">
         <v>0.15583156000000001</v>
       </c>
-      <c r="G40">
+      <c r="G40" s="10">
         <v>0.62237699999999996</v>
       </c>
-      <c r="I40">
+      <c r="I40" s="10">
         <v>5</v>
       </c>
-      <c r="J40">
+      <c r="J40" s="10">
         <v>2.4147228736378299</v>
       </c>
-      <c r="K40">
+      <c r="K40" s="10">
         <v>2.41243006221181</v>
       </c>
     </row>
     <row r="41" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A41">
+      <c r="A41" s="10">
         <v>7</v>
       </c>
-      <c r="B41">
+      <c r="B41" s="10">
         <v>1.9696094</v>
       </c>
-      <c r="C41">
+      <c r="C41" s="10">
         <v>1.9570471</v>
       </c>
-      <c r="E41">
+      <c r="E41" s="10">
         <v>7</v>
       </c>
-      <c r="F41">
+      <c r="F41" s="10">
         <v>0.21362929</v>
       </c>
-      <c r="G41">
+      <c r="G41" s="10">
         <v>0.21310903</v>
       </c>
-      <c r="I41">
+      <c r="I41" s="10">
         <v>6</v>
       </c>
-      <c r="J41">
+      <c r="J41" s="10">
         <v>1.96151016800439</v>
       </c>
-      <c r="K41">
+      <c r="K41" s="10">
         <v>1.95793523173706</v>
       </c>
     </row>
     <row r="42" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A42">
+      <c r="A42" s="10">
         <v>7.25</v>
       </c>
-      <c r="B42">
+      <c r="B42" s="10">
         <v>1.7583034</v>
       </c>
-      <c r="C42">
+      <c r="C42" s="10">
         <v>1.6950942</v>
       </c>
-      <c r="E42">
+      <c r="E42" s="10">
         <v>7.25</v>
       </c>
-      <c r="F42">
+      <c r="F42" s="10">
         <v>0.73157704000000001</v>
       </c>
-      <c r="G42">
+      <c r="G42" s="10">
         <v>0.63940960000000002</v>
       </c>
-      <c r="I42">
+      <c r="I42" s="10">
         <v>7</v>
       </c>
-      <c r="J42">
+      <c r="J42" s="10">
         <v>1.7291236438909099</v>
       </c>
-      <c r="K42">
+      <c r="K42" s="10">
         <v>1.3386346607770601</v>
       </c>
     </row>
     <row r="43" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A43">
+      <c r="A43" s="10">
         <v>7.5</v>
       </c>
-      <c r="B43">
+      <c r="B43" s="10">
         <v>0.79624899999999998</v>
       </c>
-      <c r="C43">
+      <c r="C43" s="10">
         <v>0.68132037000000001</v>
       </c>
-      <c r="E43">
+      <c r="E43" s="10">
         <v>7.5</v>
       </c>
-      <c r="F43">
+      <c r="F43" s="10">
         <v>1.1253985</v>
       </c>
-      <c r="G43">
+      <c r="G43" s="10">
         <v>1.0829565999999999</v>
       </c>
-      <c r="I43">
+      <c r="I43" s="10">
         <v>8</v>
       </c>
-      <c r="J43">
+      <c r="J43" s="10">
         <v>1.0736310372529201</v>
       </c>
-      <c r="K43">
+      <c r="K43" s="10">
         <v>1.0414586716202101</v>
       </c>
     </row>
     <row r="44" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A44">
+      <c r="A44" s="10">
         <v>7.75</v>
       </c>
-      <c r="B44">
+      <c r="B44" s="10">
         <v>1.3584377000000001</v>
       </c>
-      <c r="C44">
+      <c r="C44" s="10">
         <v>0.75090559999999995</v>
       </c>
-      <c r="E44">
+      <c r="E44" s="10">
         <v>7.75</v>
       </c>
-      <c r="F44">
+      <c r="F44" s="10">
         <v>1.5985924</v>
       </c>
-      <c r="G44">
+      <c r="G44" s="10">
         <v>1.3043115999999999</v>
       </c>
-      <c r="I44">
+      <c r="I44" s="10">
         <v>9</v>
       </c>
-      <c r="J44">
+      <c r="J44" s="10">
         <v>0.59936217387988899</v>
       </c>
-      <c r="K44">
+      <c r="K44" s="10">
         <v>0.51741004930856604</v>
       </c>
     </row>
     <row r="45" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A45">
+      <c r="A45" s="10">
         <v>8</v>
       </c>
-      <c r="B45">
+      <c r="B45" s="10">
         <v>1.7966605</v>
       </c>
-      <c r="C45">
+      <c r="C45" s="10">
         <v>1.1274599000000001</v>
       </c>
-      <c r="E45">
+      <c r="E45" s="10">
         <v>8</v>
       </c>
-      <c r="F45">
+      <c r="F45" s="10">
         <v>1.9290111999999999</v>
       </c>
-      <c r="G45">
+      <c r="G45" s="10">
         <v>0.93027203999999997</v>
       </c>
-      <c r="I45">
+      <c r="I45" s="10">
         <v>10</v>
       </c>
-      <c r="J45">
+      <c r="J45" s="10">
         <v>0.29911634894509698</v>
       </c>
-      <c r="K45">
+      <c r="K45" s="10">
         <v>0.233693339719897</v>
       </c>
     </row>
     <row r="46" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A46">
+      <c r="A46" s="10">
         <v>8.25</v>
       </c>
-      <c r="B46">
+      <c r="B46" s="10">
         <v>1.973624</v>
       </c>
-      <c r="C46">
+      <c r="C46" s="10">
         <v>1.4339782000000001</v>
       </c>
-      <c r="E46">
+      <c r="E46" s="10">
         <v>8.25</v>
       </c>
-      <c r="F46">
+      <c r="F46" s="10">
         <v>1.9670014</v>
       </c>
-      <c r="G46">
+      <c r="G46" s="10">
         <v>0.92098146999999997</v>
       </c>
     </row>
     <row r="47" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A47">
+      <c r="A47" s="10">
         <v>8.5</v>
       </c>
-      <c r="B47">
+      <c r="B47" s="10">
         <v>1.9196076</v>
       </c>
-      <c r="C47">
+      <c r="C47" s="10">
         <v>0.87702124999999997</v>
       </c>
-      <c r="E47">
+      <c r="E47" s="10">
         <v>8.5</v>
       </c>
-      <c r="F47">
+      <c r="F47" s="10">
         <v>1.8652599999999999</v>
       </c>
-      <c r="G47">
+      <c r="G47" s="10">
         <v>0.95180900000000002</v>
       </c>
-      <c r="I47" s="3" t="s">
+      <c r="I47" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="J47" s="6" t="s">
+      <c r="J47" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="K47" s="6" t="s">
+      <c r="K47" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="M47" t="s">
+      <c r="M47" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="N47" s="6" t="s">
+      <c r="N47" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="O47" s="6" t="s">
+      <c r="O47" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="Q47" t="s">
+      <c r="Q47" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="R47" s="6" t="s">
+      <c r="R47" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="S47" s="6" t="s">
+      <c r="S47" s="10" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="48" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A48">
+      <c r="A48" s="10">
         <v>8.75</v>
       </c>
-      <c r="B48">
+      <c r="B48" s="10">
         <v>1.9437951</v>
       </c>
-      <c r="C48">
+      <c r="C48" s="10">
         <v>1.2623333999999999</v>
       </c>
-      <c r="E48">
+      <c r="E48" s="10">
         <v>8.75</v>
       </c>
-      <c r="F48">
+      <c r="F48" s="10">
         <v>1.8260812</v>
       </c>
-      <c r="G48">
+      <c r="G48" s="10">
         <v>0.9494937</v>
       </c>
-      <c r="I48">
+      <c r="I48" s="10">
         <v>1</v>
       </c>
-      <c r="J48">
+      <c r="J48" s="10">
         <v>2.40772858268712</v>
       </c>
-      <c r="K48">
+      <c r="K48" s="10">
         <v>2.4074556325173799</v>
       </c>
-      <c r="M48" s="6" t="s">
+      <c r="M48" s="10" t="s">
         <v>16</v>
       </c>
       <c r="N48" s="10">
@@ -33027,10 +33025,10 @@
       <c r="O48" s="10">
         <v>16.149999999999999</v>
       </c>
-      <c r="Q48" s="6" t="s">
+      <c r="Q48" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="R48" s="12">
+      <c r="R48" s="10">
         <v>1</v>
       </c>
       <c r="S48" s="10">
@@ -33038,34 +33036,34 @@
       </c>
     </row>
     <row r="49" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A49">
+      <c r="A49" s="10">
         <v>9</v>
       </c>
-      <c r="B49">
+      <c r="B49" s="10">
         <v>1.9199132999999999</v>
       </c>
-      <c r="C49">
+      <c r="C49" s="10">
         <v>0.83831670000000003</v>
       </c>
-      <c r="E49">
+      <c r="E49" s="10">
         <v>9</v>
       </c>
-      <c r="F49">
+      <c r="F49" s="10">
         <v>1.9433838000000001</v>
       </c>
-      <c r="G49">
+      <c r="G49" s="10">
         <v>0.97163193999999997</v>
       </c>
-      <c r="I49">
+      <c r="I49" s="10">
         <v>2</v>
       </c>
-      <c r="J49">
+      <c r="J49" s="10">
         <v>2.40382888512034</v>
       </c>
-      <c r="K49">
+      <c r="K49" s="10">
         <v>2.4014276030405299</v>
       </c>
-      <c r="M49" s="6" t="s">
+      <c r="M49" s="10" t="s">
         <v>17</v>
       </c>
       <c r="N49" s="10">
@@ -33074,200 +33072,199 @@
       <c r="O49" s="10">
         <v>0</v>
       </c>
-      <c r="P49" s="10"/>
-      <c r="Q49" s="6" t="s">
+      <c r="Q49" s="10" t="s">
         <v>17</v>
       </c>
       <c r="R49" s="10">
         <v>8.7319999999999997E-5</v>
       </c>
-      <c r="S49" s="13">
+      <c r="S49" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A50">
+      <c r="A50" s="10">
         <v>9.25</v>
       </c>
-      <c r="B50">
+      <c r="B50" s="10">
         <v>1.8697569999999999</v>
       </c>
-      <c r="C50">
+      <c r="C50" s="10">
         <v>1.2153125</v>
       </c>
-      <c r="E50">
+      <c r="E50" s="10">
         <v>9.25</v>
       </c>
-      <c r="F50">
+      <c r="F50" s="10">
         <v>0.86561924000000001</v>
       </c>
-      <c r="G50">
+      <c r="G50" s="10">
         <v>0.80045825000000004</v>
       </c>
-      <c r="I50">
+      <c r="I50" s="10">
         <v>3</v>
       </c>
-      <c r="J50" s="4">
+      <c r="J50" s="10">
         <v>2.4010104043791101</v>
       </c>
-      <c r="K50">
+      <c r="K50" s="10">
         <v>2.3948106423125899</v>
       </c>
     </row>
     <row r="51" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A51">
+      <c r="A51" s="10">
         <v>9.5</v>
       </c>
-      <c r="B51">
+      <c r="B51" s="10">
         <v>1.393645</v>
       </c>
-      <c r="C51">
+      <c r="C51" s="10">
         <v>1.0550021000000001</v>
       </c>
-      <c r="E51">
+      <c r="E51" s="10">
         <v>9.5</v>
       </c>
-      <c r="F51">
+      <c r="F51" s="10">
         <v>1.3593689</v>
       </c>
-      <c r="G51">
+      <c r="G51" s="10">
         <v>0.66504399999999997</v>
       </c>
-      <c r="I51">
+      <c r="I51" s="10">
         <v>4</v>
       </c>
-      <c r="J51">
+      <c r="J51" s="10">
         <v>2.3961440432977499</v>
       </c>
-      <c r="K51">
+      <c r="K51" s="10">
         <v>2.3876217050610999</v>
       </c>
     </row>
     <row r="52" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A52">
+      <c r="A52" s="10">
         <v>9.75</v>
       </c>
-      <c r="B52">
+      <c r="B52" s="10">
         <v>1.0465989</v>
       </c>
-      <c r="C52">
+      <c r="C52" s="10">
         <v>1.069291</v>
       </c>
-      <c r="E52">
+      <c r="E52" s="10">
         <v>9.75</v>
       </c>
-      <c r="F52">
+      <c r="F52" s="10">
         <v>1.7986660999999999</v>
       </c>
-      <c r="G52">
+      <c r="G52" s="10">
         <v>0.74505560000000004</v>
       </c>
-      <c r="I52">
+      <c r="I52" s="10">
         <v>5</v>
       </c>
-      <c r="J52">
+      <c r="J52" s="10">
         <v>2.3386448247934299</v>
       </c>
-      <c r="K52">
+      <c r="K52" s="10">
         <v>2.3380419708430802</v>
       </c>
     </row>
     <row r="53" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="I53">
+      <c r="I53" s="10">
         <v>6</v>
       </c>
-      <c r="J53">
+      <c r="J53" s="10">
         <v>1.9716103621054999</v>
       </c>
-      <c r="K53">
+      <c r="K53" s="10">
         <v>1.8617380009025699</v>
       </c>
     </row>
     <row r="54" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="I54">
+      <c r="I54" s="10">
         <v>7</v>
       </c>
-      <c r="J54">
+      <c r="J54" s="10">
         <v>1.5097331919243699</v>
       </c>
-      <c r="K54">
+      <c r="K54" s="10">
         <v>1.4040843303577799</v>
       </c>
     </row>
     <row r="55" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="I55">
+      <c r="I55" s="10">
         <v>8</v>
       </c>
-      <c r="J55">
+      <c r="J55" s="10">
         <v>1.0685105775080499</v>
       </c>
-      <c r="K55">
+      <c r="K55" s="10">
         <v>0.90412141379983901</v>
       </c>
     </row>
     <row r="56" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="I56">
+      <c r="I56" s="10">
         <v>9</v>
       </c>
-      <c r="J56">
+      <c r="J56" s="10">
         <v>0.625007323845163</v>
       </c>
-      <c r="K56">
+      <c r="K56" s="10">
         <v>0.55883012125238096</v>
       </c>
     </row>
     <row r="57" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="I57">
+      <c r="I57" s="10">
         <v>10</v>
       </c>
-      <c r="J57">
+      <c r="J57" s="10">
         <v>0.415025755405944</v>
       </c>
-      <c r="K57">
+      <c r="K57" s="10">
         <v>0.28542641071339803</v>
       </c>
     </row>
     <row r="59" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="I59" s="3" t="s">
+      <c r="I59" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="J59" s="6" t="s">
+      <c r="J59" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="K59" s="6" t="s">
+      <c r="K59" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="M59" t="s">
+      <c r="M59" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="N59" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="O59" s="6" t="s">
+      <c r="N59" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="O59" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="Q59" t="s">
+      <c r="Q59" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="R59" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="S59" s="6" t="s">
-        <v>17</v>
+      <c r="R59" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="S59" s="10" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="60" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="I60">
+      <c r="I60" s="10">
         <v>1</v>
       </c>
-      <c r="J60">
+      <c r="J60" s="10">
         <v>2.5532883846338899</v>
       </c>
-      <c r="K60">
+      <c r="K60" s="10">
         <v>2.5529877249322501</v>
       </c>
-      <c r="M60" s="6" t="s">
-        <v>16</v>
+      <c r="M60" s="10" t="s">
+        <v>11</v>
       </c>
       <c r="N60" s="10">
         <v>0</v>
@@ -33275,10 +33272,10 @@
       <c r="O60" s="10">
         <v>17.963999999999999</v>
       </c>
-      <c r="Q60" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="R60" s="12">
+      <c r="Q60" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="R60" s="10">
         <v>1</v>
       </c>
       <c r="S60" s="10">
@@ -33286,17 +33283,17 @@
       </c>
     </row>
     <row r="61" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="I61">
+      <c r="I61" s="10">
         <v>2</v>
       </c>
-      <c r="J61">
+      <c r="J61" s="10">
         <v>2.5505554074535102</v>
       </c>
-      <c r="K61">
+      <c r="K61" s="10">
         <v>2.5477398997380298</v>
       </c>
-      <c r="M61" s="6" t="s">
-        <v>17</v>
+      <c r="M61" s="10" t="s">
+        <v>3</v>
       </c>
       <c r="N61" s="10">
         <v>17.963999999999999</v>
@@ -33304,102 +33301,101 @@
       <c r="O61" s="10">
         <v>0</v>
       </c>
-      <c r="P61" s="10"/>
-      <c r="Q61" s="6" t="s">
+      <c r="Q61" s="10" t="s">
         <v>17</v>
       </c>
       <c r="R61" s="10">
         <v>1.48858E-4</v>
       </c>
-      <c r="S61" s="13">
+      <c r="S61" s="10">
         <v>1</v>
       </c>
     </row>
     <row r="62" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="I62">
+      <c r="I62" s="10">
         <v>3</v>
       </c>
-      <c r="J62">
+      <c r="J62" s="10">
         <v>2.54535181894718</v>
       </c>
-      <c r="K62">
+      <c r="K62" s="10">
         <v>2.5435855958671199</v>
       </c>
     </row>
     <row r="63" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="I63">
+      <c r="I63" s="10">
         <v>4</v>
       </c>
-      <c r="J63">
+      <c r="J63" s="10">
         <v>2.53772691465291</v>
       </c>
-      <c r="K63">
+      <c r="K63" s="10">
         <v>2.5365997228625901</v>
       </c>
     </row>
     <row r="64" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="I64">
+      <c r="I64" s="10">
         <v>5</v>
       </c>
-      <c r="J64">
+      <c r="J64" s="10">
         <v>2.4147228736378299</v>
       </c>
-      <c r="K64">
+      <c r="K64" s="10">
         <v>2.41243006221181</v>
       </c>
     </row>
     <row r="65" spans="9:11" x14ac:dyDescent="0.25">
-      <c r="I65">
+      <c r="I65" s="10">
         <v>6</v>
       </c>
-      <c r="J65">
+      <c r="J65" s="10">
         <v>1.96151016800439</v>
       </c>
-      <c r="K65">
+      <c r="K65" s="10">
         <v>1.95793523173706</v>
       </c>
     </row>
     <row r="66" spans="9:11" x14ac:dyDescent="0.25">
-      <c r="I66">
+      <c r="I66" s="10">
         <v>7</v>
       </c>
-      <c r="J66">
+      <c r="J66" s="10">
         <v>1.7291236438909099</v>
       </c>
-      <c r="K66">
+      <c r="K66" s="10">
         <v>1.3386346607770601</v>
       </c>
     </row>
     <row r="67" spans="9:11" x14ac:dyDescent="0.25">
-      <c r="I67">
+      <c r="I67" s="10">
         <v>8</v>
       </c>
-      <c r="J67">
+      <c r="J67" s="10">
         <v>1.0736310372529201</v>
       </c>
-      <c r="K67">
+      <c r="K67" s="10">
         <v>1.0414586716202101</v>
       </c>
     </row>
     <row r="68" spans="9:11" x14ac:dyDescent="0.25">
-      <c r="I68">
+      <c r="I68" s="10">
         <v>9</v>
       </c>
-      <c r="J68">
+      <c r="J68" s="10">
         <v>0.59936217387988899</v>
       </c>
-      <c r="K68">
+      <c r="K68" s="10">
         <v>0.51741004930856604</v>
       </c>
     </row>
     <row r="69" spans="9:11" x14ac:dyDescent="0.25">
-      <c r="I69">
+      <c r="I69" s="10">
         <v>10</v>
       </c>
-      <c r="J69">
+      <c r="J69" s="10">
         <v>0.29911634894509698</v>
       </c>
-      <c r="K69">
+      <c r="K69" s="10">
         <v>0.233693339719897</v>
       </c>
     </row>

</xml_diff>